<commit_message>
assessment template latest and fixes
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/assessment/002_EAC_Assessment.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/assessment/002_EAC_Assessment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\epic\track\code\epictrack-api\src\api\templates\event_templates\assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8339129A-04FB-4388-9E41-FD0277AB39DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F32154-305A-49FA-AB56-9C730B9C82B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phases" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Actions!$D$1:$D$257</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Events!$A$1:$M$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Events!$A$1:$M$337</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Outcomes!$A$1:$E$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2477" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2478" uniqueCount="396">
   <si>
     <t>No</t>
   </si>
@@ -1229,6 +1229,9 @@
   </si>
   <si>
     <t>[{"phase_name":"Pre-EA (EAC Assessment)","work_type_id": 6, "ea_act_id": 3, "event_name": "Submission of IPD/EP for CEAO Approval", "start_at": 28 },{"phase_name":"Pre-EA (EAC Assessment)","work_type_id": 6, "ea_act_id": 3, "event_name": "IPD/EP Approval Decision (Day Zero)", "start_at": 10 }]</t>
+  </si>
+  <si>
+    <t>TESTED</t>
   </si>
 </sst>
 </file>
@@ -1342,7 +1345,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1448,6 +1451,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFE2EFDA"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1562,7 +1571,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1760,6 +1769,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3095,11 +3107,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M337"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B139" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D137" sqref="A137:D137"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -16781,7 +16793,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M71" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <autoFilter ref="A1:M337" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <conditionalFormatting sqref="H1:H16 H18:H337">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="END">
       <formula>NOT(ISERROR(SEARCH("END",H1)))</formula>
@@ -16838,13 +16850,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A37" sqref="A37:D66"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -16856,7 +16868,7 @@
     <col min="6" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1">
+    <row r="1" spans="1:6" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -16872,8 +16884,11 @@
       <c r="E1" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="6" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -16891,7 +16906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -16909,7 +16924,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -16927,7 +16942,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -16945,7 +16960,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -16962,8 +16977,9 @@
       <c r="E6" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" s="69"/>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -16981,7 +16997,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -16999,7 +17015,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -17017,7 +17033,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -17035,7 +17051,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -17053,7 +17069,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -17071,7 +17087,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -17089,7 +17105,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -17107,7 +17123,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:6">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -17125,7 +17141,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -18065,11 +18081,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F8" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -24703,12 +24719,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -24941,20 +24959,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37DBE489-EE2E-427D-B9CD-0FAE2F0995FB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0BEEB2-93D8-45BE-86D5-11172DAC5CD0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
+    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -24979,12 +24998,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0BEEB2-93D8-45BE-86D5-11172DAC5CD0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37DBE489-EE2E-427D-B9CD-0FAE2F0995FB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
-    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
assessment template related fixes
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/assessment/002_EAC_Assessment.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/assessment/002_EAC_Assessment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\epic\track\code\epictrack-api\src\api\templates\event_templates\assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F32154-305A-49FA-AB56-9C730B9C82B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE9D403-7FF9-4851-940F-D598A8ADAB1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phases" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2478" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2478" uniqueCount="395">
   <si>
     <t>No</t>
   </si>
@@ -1141,9 +1141,6 @@
     <t>{"start_date_locked": true}</t>
   </si>
   <si>
-    <t>{"phase_name":"Early Engagement","work_type_id": 6, "ea_act_id": 3, "event_name": "IPD/EP Approved (Day One)", "start_at": 28 }</t>
-  </si>
-  <si>
     <t>{"phase_name":"Revised EAC Application Development (Proponent Time)","work_type_id": 6, "ea_act_id": 3, "event_name": "Start of Revised EAC Application Development", "start_at": 1 }</t>
   </si>
   <si>
@@ -1210,9 +1207,6 @@
     <t>Add PHASE "Revised DPD Development (Proponent Time)" (a renamed copy of original PHASE),Add PHASE "Readiness Decision" (a copy of original PHASE)</t>
   </si>
   <si>
-    <t>[{"phase_name":"DPD Development (Proponent Time)","work_type_id": 6, "ea_act_id": 3, "new_name": "Revised DPD Development (Proponent Time)", "legislated": false },{"phase_name":"Readiness Decision","work_type_id": 6, "ea_act_id": 3, "new_name": "Revised Readiness Decision", "legislated": false }]</t>
-  </si>
-  <si>
     <t>[{"phase_name":"DPD Development (Proponent Time)","work_type_id": 6, "ea_act_id": 3, "new_name": "Revised DPD Development (Proponent Time)", "legislated": false },{"phase_name":"Readiness Decision","work_type_id": 6, "ea_act_id": 3, "new_name": "Readiness Decision", "legislated": false }]</t>
   </si>
   <si>
@@ -1232,18 +1226,28 @@
   </si>
   <si>
     <t>TESTED</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Early Engagement","work_type_id": 6, "ea_act_id": 3, "event_name": "IPD/EP Approved (Day One)", "start_at": 1 }</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1571,7 +1575,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1588,14 +1592,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1604,7 +1608,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1616,19 +1620,19 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1637,22 +1641,22 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1697,7 +1701,7 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1721,45 +1725,48 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1768,10 +1775,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2136,7 +2143,7 @@
         <v>304</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>9</v>
@@ -2165,7 +2172,7 @@
         <v>152</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>9</v>
@@ -2194,7 +2201,7 @@
         <v>153</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>9</v>
@@ -2223,7 +2230,7 @@
         <v>154</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>9</v>
@@ -2252,7 +2259,7 @@
         <v>155</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>9</v>
@@ -2281,7 +2288,7 @@
         <v>156</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>9</v>
@@ -2310,7 +2317,7 @@
         <v>157</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>9</v>
@@ -2339,7 +2346,7 @@
         <v>158</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>9</v>
@@ -2368,7 +2375,7 @@
         <v>159</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>9</v>
@@ -2397,7 +2404,7 @@
         <v>160</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>9</v>
@@ -2426,7 +2433,7 @@
         <v>161</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>9</v>
@@ -2455,7 +2462,7 @@
         <v>162</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>9</v>
@@ -3107,11 +3114,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M337"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -16852,11 +16859,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomRight" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -16885,7 +16892,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -17032,6 +17039,7 @@
       <c r="E9" s="2">
         <v>8</v>
       </c>
+      <c r="F9" s="69"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="2">
@@ -17050,6 +17058,7 @@
       <c r="E10" s="2">
         <v>9</v>
       </c>
+      <c r="F10" s="69"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="2">
@@ -17062,12 +17071,13 @@
         <f>IF((B11=""),"",VLOOKUP(B11,Events!$A$2:$D$336,4,FALSE))</f>
         <v>IPD/EP Approval Decision (Day Zero)</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="70" t="s">
         <v>271</v>
       </c>
       <c r="E11" s="2">
         <v>10</v>
       </c>
+      <c r="F11" s="69"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="2">
@@ -17159,7 +17169,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -17177,7 +17187,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:6">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -17195,7 +17205,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:6">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -17213,7 +17223,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:6">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -17231,7 +17241,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:6">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -17249,7 +17259,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:6">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -17266,8 +17276,9 @@
       <c r="E22" s="2">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22" s="69"/>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -17285,7 +17296,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:6">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -17296,14 +17307,15 @@
         <f>IF((B24=""),"",VLOOKUP(B24,Events!$A$2:$D$336,4,FALSE))</f>
         <v>CEAO's Readiness Decision (EAC Assessment)</v>
       </c>
-      <c r="D24" s="26" t="s">
+      <c r="D24" s="70" t="s">
         <v>273</v>
       </c>
       <c r="E24" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24" s="69"/>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -17314,14 +17326,15 @@
         <f>IF((B25=""),"",VLOOKUP(B25,Events!$A$2:$D$336,4,FALSE))</f>
         <v>CEAO's Readiness Decision (EAC Assessment)</v>
       </c>
-      <c r="D25" s="26" t="s">
+      <c r="D25" s="70" t="s">
         <v>274</v>
       </c>
       <c r="E25" s="2">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25" s="69"/>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -17332,14 +17345,14 @@
         <f>IF((B26=""),"",VLOOKUP(B26,Events!$A$2:$D$336,4,FALSE))</f>
         <v>CEAO's Readiness Decision (EAC Assessment)</v>
       </c>
-      <c r="D26" s="26" t="s">
+      <c r="D26" s="70" t="s">
         <v>277</v>
       </c>
       <c r="E26" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:6">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -17357,7 +17370,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:6">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -17375,7 +17388,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:6">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -17393,7 +17406,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:6">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -17411,7 +17424,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:6">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -17429,7 +17442,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:6">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -18082,10 +18095,10 @@
   <dimension ref="A1:G257"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomRight" activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -18141,7 +18154,7 @@
         <v>297</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G2" s="2">
         <v>1</v>
@@ -18573,7 +18586,7 @@
         <v>312</v>
       </c>
       <c r="F20" s="66" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G20" s="2">
         <v>19</v>
@@ -18597,7 +18610,7 @@
         <v>297</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G21" s="2">
         <v>20</v>
@@ -18621,7 +18634,7 @@
         <v>297</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G22" s="2">
         <v>21</v>
@@ -18765,7 +18778,7 @@
         <v>315</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>365</v>
+        <v>394</v>
       </c>
       <c r="G28" s="2">
         <v>27</v>
@@ -18786,10 +18799,10 @@
         <v>85</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="G29" s="2">
         <v>28</v>
@@ -18810,10 +18823,10 @@
         <v>88</v>
       </c>
       <c r="E30" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>384</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>385</v>
       </c>
       <c r="G30" s="2">
         <v>29</v>
@@ -19053,7 +19066,7 @@
         <v>317</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G40" s="2">
         <v>39</v>
@@ -19077,7 +19090,7 @@
         <v>297</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G41" s="2">
         <v>40</v>
@@ -19101,7 +19114,7 @@
         <v>297</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G42" s="2">
         <v>41</v>
@@ -19554,10 +19567,10 @@
         <v>97</v>
       </c>
       <c r="E61" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F61" s="70" t="s">
         <v>387</v>
-      </c>
-      <c r="F61" s="68" t="s">
-        <v>388</v>
       </c>
       <c r="G61" s="2">
         <v>60</v>
@@ -19581,7 +19594,7 @@
         <v>319</v>
       </c>
       <c r="F62" s="66" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G62" s="2">
         <v>61</v>
@@ -19605,7 +19618,7 @@
         <v>322</v>
       </c>
       <c r="F63" s="66" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G63" s="2">
         <v>62</v>
@@ -19629,7 +19642,7 @@
         <v>324</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G64" s="2">
         <v>63</v>
@@ -19653,7 +19666,7 @@
         <v>325</v>
       </c>
       <c r="F65" s="66" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G65" s="2">
         <v>64</v>
@@ -19677,7 +19690,7 @@
         <v>326</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G66" s="2">
         <v>65</v>
@@ -19701,7 +19714,7 @@
         <v>327</v>
       </c>
       <c r="F67" s="66" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G67" s="2">
         <v>66</v>
@@ -19725,7 +19738,7 @@
         <v>328</v>
       </c>
       <c r="F68" s="66" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G68" s="2">
         <v>67</v>
@@ -19749,7 +19762,7 @@
         <v>329</v>
       </c>
       <c r="F69" s="66" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G69" s="2">
         <v>68</v>
@@ -19773,7 +19786,7 @@
         <v>334</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G70" s="2">
         <v>69</v>
@@ -20061,7 +20074,7 @@
         <v>330</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G82" s="2">
         <v>81</v>
@@ -20085,7 +20098,7 @@
         <v>331</v>
       </c>
       <c r="F83" s="66" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G83" s="2">
         <v>82</v>
@@ -20298,10 +20311,10 @@
         <v>97</v>
       </c>
       <c r="E92" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F92" s="1" t="s">
         <v>387</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>389</v>
       </c>
       <c r="G92" s="2">
         <v>91</v>
@@ -20325,7 +20338,7 @@
         <v>319</v>
       </c>
       <c r="F93" s="66" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G93" s="2">
         <v>92</v>
@@ -20349,7 +20362,7 @@
         <v>322</v>
       </c>
       <c r="F94" s="66" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G94" s="2">
         <v>93</v>
@@ -20373,7 +20386,7 @@
         <v>329</v>
       </c>
       <c r="F95" s="66" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G95" s="2">
         <v>94</v>
@@ -20397,7 +20410,7 @@
         <v>334</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G96" s="2">
         <v>95</v>
@@ -20421,7 +20434,7 @@
         <v>332</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G97" s="2">
         <v>96</v>
@@ -20445,7 +20458,7 @@
         <v>333</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G98" s="2">
         <v>97</v>
@@ -20469,7 +20482,7 @@
         <v>334</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G99" s="2">
         <v>98</v>
@@ -20733,7 +20746,7 @@
         <v>297</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G110" s="2">
         <v>109</v>
@@ -20757,7 +20770,7 @@
         <v>297</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G111" s="2">
         <v>110</v>
@@ -21213,7 +21226,7 @@
         <v>312</v>
       </c>
       <c r="F130" s="66" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G130" s="2">
         <v>129</v>
@@ -21237,7 +21250,7 @@
         <v>297</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G131" s="2">
         <v>130</v>
@@ -21261,7 +21274,7 @@
         <v>297</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G132" s="2">
         <v>131</v>
@@ -21501,7 +21514,7 @@
         <v>336</v>
       </c>
       <c r="F142" s="66" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G142" s="2">
         <v>141</v>
@@ -21522,10 +21535,10 @@
         <v>85</v>
       </c>
       <c r="E143" s="68" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="G143" s="2">
         <v>142</v>
@@ -21549,7 +21562,7 @@
         <v>337</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G144" s="2">
         <v>143</v>
@@ -21789,7 +21802,7 @@
         <v>340</v>
       </c>
       <c r="F154" s="66" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G154" s="2">
         <v>153</v>
@@ -21933,7 +21946,7 @@
         <v>342</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G160" s="2">
         <v>159</v>
@@ -23269,7 +23282,7 @@
     </row>
     <row r="6" spans="1:59">
       <c r="B6" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>24</v>
@@ -24719,14 +24732,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -24959,21 +24970,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0BEEB2-93D8-45BE-86D5-11172DAC5CD0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37DBE489-EE2E-427D-B9CD-0FAE2F0995FB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
-    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -24998,9 +25008,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37DBE489-EE2E-427D-B9CD-0FAE2F0995FB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0BEEB2-93D8-45BE-86D5-11172DAC5CD0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
+    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Assessment latest template related fixes (#2012)
* actual date max value for extension event

* fixes

* assessment template latest and fixes

* assessment template related fixes
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/assessment/002_EAC_Assessment.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/assessment/002_EAC_Assessment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\epic\track\code\epictrack-api\src\api\templates\event_templates\assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F32154-305A-49FA-AB56-9C730B9C82B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D598A7FB-D144-4454-9B35-0D4BD8F73DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phases" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2478" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2471" uniqueCount="394">
   <si>
     <t>No</t>
   </si>
@@ -931,9 +931,6 @@
     <t>Environmental Assessment Certificate REFUSED</t>
   </si>
   <si>
-    <t>======================================================================</t>
-  </si>
-  <si>
     <t>NONE</t>
   </si>
   <si>
@@ -1141,9 +1138,6 @@
     <t>{"start_date_locked": true}</t>
   </si>
   <si>
-    <t>{"phase_name":"Early Engagement","work_type_id": 6, "ea_act_id": 3, "event_name": "IPD/EP Approved (Day One)", "start_at": 28 }</t>
-  </si>
-  <si>
     <t>{"phase_name":"Revised EAC Application Development (Proponent Time)","work_type_id": 6, "ea_act_id": 3, "event_name": "Start of Revised EAC Application Development", "start_at": 1 }</t>
   </si>
   <si>
@@ -1210,9 +1204,6 @@
     <t>Add PHASE "Revised DPD Development (Proponent Time)" (a renamed copy of original PHASE),Add PHASE "Readiness Decision" (a copy of original PHASE)</t>
   </si>
   <si>
-    <t>[{"phase_name":"DPD Development (Proponent Time)","work_type_id": 6, "ea_act_id": 3, "new_name": "Revised DPD Development (Proponent Time)", "legislated": false },{"phase_name":"Readiness Decision","work_type_id": 6, "ea_act_id": 3, "new_name": "Revised Readiness Decision", "legislated": false }]</t>
-  </si>
-  <si>
     <t>[{"phase_name":"DPD Development (Proponent Time)","work_type_id": 6, "ea_act_id": 3, "new_name": "Revised DPD Development (Proponent Time)", "legislated": false },{"phase_name":"Readiness Decision","work_type_id": 6, "ea_act_id": 3, "new_name": "Readiness Decision", "legislated": false }]</t>
   </si>
   <si>
@@ -1232,18 +1223,28 @@
   </si>
   <si>
     <t>TESTED</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Early Engagement","work_type_id": 6, "ea_act_id": 3, "event_name": "IPD/EP Approved (Day One)", "start_at": 1 }</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1571,7 +1572,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1588,14 +1589,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1604,7 +1605,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1616,19 +1617,19 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1637,22 +1638,22 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1697,7 +1698,7 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1721,45 +1722,48 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1768,10 +1772,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2133,10 +2137,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="62" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>9</v>
@@ -2165,7 +2169,7 @@
         <v>152</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>9</v>
@@ -2194,7 +2198,7 @@
         <v>153</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>9</v>
@@ -2223,7 +2227,7 @@
         <v>154</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>9</v>
@@ -2252,7 +2256,7 @@
         <v>155</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>9</v>
@@ -2281,7 +2285,7 @@
         <v>156</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>9</v>
@@ -2310,7 +2314,7 @@
         <v>157</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>9</v>
@@ -2339,7 +2343,7 @@
         <v>158</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>9</v>
@@ -2368,7 +2372,7 @@
         <v>159</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>9</v>
@@ -2397,7 +2401,7 @@
         <v>160</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>9</v>
@@ -2426,7 +2430,7 @@
         <v>161</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>9</v>
@@ -2455,7 +2459,7 @@
         <v>162</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>9</v>
@@ -3107,11 +3111,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M337"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -3777,10 +3781,10 @@
         <v>1</v>
       </c>
       <c r="D17" s="63" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E17" s="64" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F17" s="65" t="s">
         <v>43</v>
@@ -6014,7 +6018,7 @@
         <v>3</v>
       </c>
       <c r="D72" s="21" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E72" s="4" t="str">
         <f>IF((C72=""),"",VLOOKUP(C72,Phases!$A$2:$B$13,2,FALSE))</f>
@@ -7552,7 +7556,7 @@
         <v>4</v>
       </c>
       <c r="D110" s="60" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E110" s="4" t="str">
         <f>IF((C110=""),"",VLOOKUP(C110,Phases!$A$2:$B$13,2,FALSE))</f>
@@ -7636,7 +7640,7 @@
         <v>4</v>
       </c>
       <c r="D112" s="22" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E112" s="4" t="str">
         <f>IF((C112=""),"",VLOOKUP(C112,Phases!$A$2:$B$13,2,FALSE))</f>
@@ -8508,7 +8512,7 @@
         <v>6</v>
       </c>
       <c r="D134" s="60" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E134" s="4" t="str">
         <f>IF((C134=""),"",VLOOKUP(C134,Phases!$A$2:$B$13,2,FALSE))</f>
@@ -8592,7 +8596,7 @@
         <v>6</v>
       </c>
       <c r="D136" s="22" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E136" s="4" t="str">
         <f>IF((C136=""),"",VLOOKUP(C136,Phases!$A$2:$B$13,2,FALSE))</f>
@@ -15990,7 +15994,7 @@
         <v>11</v>
       </c>
       <c r="D318" s="59" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E318" s="4" t="str">
         <f>IF((C318=""),"",VLOOKUP(C318,Phases!$A$2:$B$13,2,FALSE))</f>
@@ -16071,7 +16075,7 @@
         <v>12</v>
       </c>
       <c r="D320" s="58" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E320" s="4" t="str">
         <f>IF((C320=""),"",VLOOKUP(C320,Phases!$A$2:$B$13,2,FALSE))</f>
@@ -16856,7 +16860,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomRight" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -16885,7 +16889,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -16954,7 +16958,7 @@
         <v>Project Transitioning FROM the EA Act (2002)</v>
       </c>
       <c r="D5" s="55" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E5" s="2">
         <v>4</v>
@@ -16972,7 +16976,7 @@
         <v>Project Transitioning FROM the EA Act (2002)</v>
       </c>
       <c r="D6" s="55" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E6" s="2">
         <v>5</v>
@@ -17032,6 +17036,7 @@
       <c r="E9" s="2">
         <v>8</v>
       </c>
+      <c r="F9" s="69"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="2">
@@ -17050,6 +17055,7 @@
       <c r="E10" s="2">
         <v>9</v>
       </c>
+      <c r="F10" s="69"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="2">
@@ -17062,12 +17068,13 @@
         <f>IF((B11=""),"",VLOOKUP(B11,Events!$A$2:$D$336,4,FALSE))</f>
         <v>IPD/EP Approval Decision (Day Zero)</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="70" t="s">
         <v>271</v>
       </c>
       <c r="E11" s="2">
         <v>10</v>
       </c>
+      <c r="F11" s="69"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="2">
@@ -17159,7 +17166,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -17177,7 +17184,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:6">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -17195,7 +17202,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:6">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -17213,7 +17220,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:6">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -17231,7 +17238,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:6">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -17249,7 +17256,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:6">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -17266,8 +17273,9 @@
       <c r="E22" s="2">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22" s="69"/>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -17285,7 +17293,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:6">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -17296,14 +17304,15 @@
         <f>IF((B24=""),"",VLOOKUP(B24,Events!$A$2:$D$336,4,FALSE))</f>
         <v>CEAO's Readiness Decision (EAC Assessment)</v>
       </c>
-      <c r="D24" s="26" t="s">
+      <c r="D24" s="70" t="s">
         <v>273</v>
       </c>
       <c r="E24" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24" s="69"/>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -17314,14 +17323,15 @@
         <f>IF((B25=""),"",VLOOKUP(B25,Events!$A$2:$D$336,4,FALSE))</f>
         <v>CEAO's Readiness Decision (EAC Assessment)</v>
       </c>
-      <c r="D25" s="26" t="s">
+      <c r="D25" s="70" t="s">
         <v>274</v>
       </c>
       <c r="E25" s="2">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25" s="69"/>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -17332,14 +17342,14 @@
         <f>IF((B26=""),"",VLOOKUP(B26,Events!$A$2:$D$336,4,FALSE))</f>
         <v>CEAO's Readiness Decision (EAC Assessment)</v>
       </c>
-      <c r="D26" s="26" t="s">
+      <c r="D26" s="70" t="s">
         <v>277</v>
       </c>
       <c r="E26" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:6">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -17357,7 +17367,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:6">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -17375,7 +17385,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:6">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -17393,7 +17403,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:6">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -17411,7 +17421,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:6">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -17429,7 +17439,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:6">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -18081,11 +18091,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G257"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B242" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomRight" activeCell="D250" sqref="D250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -18135,13 +18145,13 @@
         <v>Assessment Transitions to the EA Act (2018) Early Engagement PHASE</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>297</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="G2" s="2">
         <v>1</v>
@@ -18162,10 +18172,10 @@
         <v>87</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G3" s="2">
         <v>2</v>
@@ -18186,10 +18196,10 @@
         <v>88</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G4" s="2">
         <v>3</v>
@@ -18210,10 +18220,10 @@
         <v>86</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G5" s="2">
         <v>4</v>
@@ -18234,10 +18244,10 @@
         <v>84</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G6" s="2">
         <v>5</v>
@@ -18258,10 +18268,10 @@
         <v>87</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G7" s="2">
         <v>6</v>
@@ -18282,10 +18292,10 @@
         <v>85</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G8" s="2">
         <v>7</v>
@@ -18306,10 +18316,10 @@
         <v>84</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G9" s="2">
         <v>8</v>
@@ -18330,10 +18340,10 @@
         <v>88</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G10" s="2">
         <v>9</v>
@@ -18354,10 +18364,10 @@
         <v>86</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="G11" s="2">
         <v>10</v>
@@ -18378,10 +18388,10 @@
         <v>84</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G12" s="2">
         <v>11</v>
@@ -18402,10 +18412,10 @@
         <v>87</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G13" s="2">
         <v>12</v>
@@ -18426,10 +18436,10 @@
         <v>88</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G14" s="2">
         <v>13</v>
@@ -18450,10 +18460,10 @@
         <v>86</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G15" s="2">
         <v>14</v>
@@ -18474,10 +18484,10 @@
         <v>84</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G16" s="2">
         <v>15</v>
@@ -18498,10 +18508,10 @@
         <v>87</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G17" s="2">
         <v>16</v>
@@ -18522,10 +18532,10 @@
         <v>88</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G18" s="2">
         <v>17</v>
@@ -18546,10 +18556,10 @@
         <v>86</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G19" s="2">
         <v>18</v>
@@ -18570,10 +18580,10 @@
         <v>84</v>
       </c>
       <c r="E20" s="66" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F20" s="66" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="G20" s="2">
         <v>19</v>
@@ -18591,13 +18601,13 @@
         <v>EAO's Viewpoint is POSITIVE</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>297</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="G21" s="2">
         <v>20</v>
@@ -18615,13 +18625,13 @@
         <v>EAO's Viewpoint is NEGATIVE</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>297</v>
-      </c>
       <c r="F22" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="G22" s="2">
         <v>21</v>
@@ -18645,7 +18655,7 @@
         <v>90</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G23" s="2">
         <v>22</v>
@@ -18669,7 +18679,7 @@
         <v>89</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G24" s="2">
         <v>23</v>
@@ -18693,7 +18703,7 @@
         <v>92</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G25" s="2">
         <v>24</v>
@@ -18714,10 +18724,10 @@
         <v>93</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G26" s="2">
         <v>25</v>
@@ -18738,10 +18748,10 @@
         <v>94</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G27" s="2">
         <v>26</v>
@@ -18762,10 +18772,10 @@
         <v>84</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>365</v>
+        <v>393</v>
       </c>
       <c r="G28" s="2">
         <v>27</v>
@@ -18786,10 +18796,10 @@
         <v>85</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="G29" s="2">
         <v>28</v>
@@ -18810,10 +18820,10 @@
         <v>88</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="G30" s="2">
         <v>29</v>
@@ -18834,10 +18844,10 @@
         <v>95</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G31" s="2">
         <v>30</v>
@@ -18861,7 +18871,7 @@
         <v>90</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G32" s="2">
         <v>31</v>
@@ -18885,7 +18895,7 @@
         <v>89</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G33" s="2">
         <v>32</v>
@@ -18909,7 +18919,7 @@
         <v>96</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G34" s="2">
         <v>33</v>
@@ -18930,10 +18940,10 @@
         <v>93</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G35" s="2">
         <v>34</v>
@@ -18957,7 +18967,7 @@
         <v>90</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G36" s="2">
         <v>35</v>
@@ -18981,7 +18991,7 @@
         <v>89</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G37" s="2">
         <v>36</v>
@@ -19005,7 +19015,7 @@
         <v>92</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G38" s="2">
         <v>37</v>
@@ -19026,10 +19036,10 @@
         <v>93</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G39" s="2">
         <v>38</v>
@@ -19050,10 +19060,10 @@
         <v>84</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="G40" s="2">
         <v>39</v>
@@ -19071,13 +19081,13 @@
         <v>EAO's Viewpoint is POSITIVE</v>
       </c>
       <c r="D41" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>297</v>
-      </c>
       <c r="F41" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="G41" s="2">
         <v>40</v>
@@ -19095,13 +19105,13 @@
         <v>EAO's Viewpoint is NEGATIVE</v>
       </c>
       <c r="D42" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="E42" s="1" t="s">
-        <v>297</v>
-      </c>
       <c r="F42" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="G42" s="2">
         <v>41</v>
@@ -19122,10 +19132,10 @@
         <v>95</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G43" s="2">
         <v>42</v>
@@ -19149,7 +19159,7 @@
         <v>90</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G44" s="2">
         <v>43</v>
@@ -19173,7 +19183,7 @@
         <v>89</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G45" s="2">
         <v>44</v>
@@ -19197,7 +19207,7 @@
         <v>96</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G46" s="2">
         <v>45</v>
@@ -19218,10 +19228,10 @@
         <v>93</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G47" s="2">
         <v>46</v>
@@ -19245,7 +19255,7 @@
         <v>90</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G48" s="2">
         <v>47</v>
@@ -19269,7 +19279,7 @@
         <v>89</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G49" s="2">
         <v>48</v>
@@ -19293,7 +19303,7 @@
         <v>92</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G50" s="2">
         <v>49</v>
@@ -19314,10 +19324,10 @@
         <v>93</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G51" s="2">
         <v>50</v>
@@ -19338,10 +19348,10 @@
         <v>95</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G52" s="2">
         <v>51</v>
@@ -19365,7 +19375,7 @@
         <v>90</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G53" s="2">
         <v>52</v>
@@ -19389,7 +19399,7 @@
         <v>89</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G54" s="2">
         <v>53</v>
@@ -19413,7 +19423,7 @@
         <v>96</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G55" s="2">
         <v>54</v>
@@ -19434,10 +19444,10 @@
         <v>93</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G56" s="2">
         <v>55</v>
@@ -19461,7 +19471,7 @@
         <v>90</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G57" s="2">
         <v>56</v>
@@ -19485,7 +19495,7 @@
         <v>89</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G58" s="2">
         <v>57</v>
@@ -19509,7 +19519,7 @@
         <v>92</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G59" s="2">
         <v>58</v>
@@ -19530,10 +19540,10 @@
         <v>93</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G60" s="2">
         <v>59</v>
@@ -19554,10 +19564,10 @@
         <v>97</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="F61" s="68" t="s">
-        <v>388</v>
+        <v>385</v>
+      </c>
+      <c r="F61" s="70" t="s">
+        <v>386</v>
       </c>
       <c r="G61" s="2">
         <v>60</v>
@@ -19578,10 +19588,10 @@
         <v>87</v>
       </c>
       <c r="E62" s="67" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F62" s="66" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="G62" s="2">
         <v>61</v>
@@ -19602,10 +19612,10 @@
         <v>84</v>
       </c>
       <c r="E63" s="66" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F63" s="66" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="G63" s="2">
         <v>62</v>
@@ -19626,10 +19636,10 @@
         <v>97</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="G64" s="2">
         <v>63</v>
@@ -19650,10 +19660,10 @@
         <v>85</v>
       </c>
       <c r="E65" s="66" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F65" s="66" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="G65" s="2">
         <v>64</v>
@@ -19674,10 +19684,10 @@
         <v>84</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="G66" s="2">
         <v>65</v>
@@ -19698,10 +19708,10 @@
         <v>84</v>
       </c>
       <c r="E67" s="66" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F67" s="66" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="G67" s="2">
         <v>66</v>
@@ -19722,10 +19732,10 @@
         <v>88</v>
       </c>
       <c r="E68" s="66" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F68" s="66" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="G68" s="2">
         <v>67</v>
@@ -19746,10 +19756,10 @@
         <v>84</v>
       </c>
       <c r="E69" s="66" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F69" s="66" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="G69" s="2">
         <v>68</v>
@@ -19767,13 +19777,13 @@
         <v>Project is Referred to Minister for Process Planning - s.18(1)(b)</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E70" s="55" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="G70" s="2">
         <v>69</v>
@@ -19797,7 +19807,7 @@
         <v>90</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G71" s="2">
         <v>70</v>
@@ -19821,7 +19831,7 @@
         <v>89</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G72" s="2">
         <v>71</v>
@@ -19845,7 +19855,7 @@
         <v>96</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G73" s="2">
         <v>72</v>
@@ -19866,10 +19876,10 @@
         <v>93</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G74" s="2">
         <v>73</v>
@@ -19893,7 +19903,7 @@
         <v>90</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G75" s="2">
         <v>74</v>
@@ -19917,7 +19927,7 @@
         <v>89</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G76" s="2">
         <v>75</v>
@@ -19941,7 +19951,7 @@
         <v>92</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G77" s="2">
         <v>76</v>
@@ -19962,10 +19972,10 @@
         <v>93</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G78" s="2">
         <v>77</v>
@@ -19989,7 +19999,7 @@
         <v>89</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G79" s="2">
         <v>78</v>
@@ -20013,7 +20023,7 @@
         <v>96</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G80" s="2">
         <v>79</v>
@@ -20034,10 +20044,10 @@
         <v>93</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G81" s="2">
         <v>80</v>
@@ -20058,10 +20068,10 @@
         <v>97</v>
       </c>
       <c r="E82" s="55" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="G82" s="2">
         <v>81</v>
@@ -20082,10 +20092,10 @@
         <v>84</v>
       </c>
       <c r="E83" s="66" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F83" s="66" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="G83" s="2">
         <v>82</v>
@@ -20109,7 +20119,7 @@
         <v>90</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G84" s="2">
         <v>83</v>
@@ -20133,7 +20143,7 @@
         <v>89</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G85" s="2">
         <v>84</v>
@@ -20157,7 +20167,7 @@
         <v>96</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G86" s="2">
         <v>85</v>
@@ -20178,10 +20188,10 @@
         <v>93</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G87" s="2">
         <v>86</v>
@@ -20205,7 +20215,7 @@
         <v>90</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G88" s="2">
         <v>87</v>
@@ -20229,7 +20239,7 @@
         <v>89</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G89" s="2">
         <v>88</v>
@@ -20253,7 +20263,7 @@
         <v>92</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G90" s="2">
         <v>89</v>
@@ -20274,10 +20284,10 @@
         <v>93</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G91" s="2">
         <v>90</v>
@@ -20298,10 +20308,10 @@
         <v>97</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="G92" s="2">
         <v>91</v>
@@ -20322,10 +20332,10 @@
         <v>87</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F93" s="66" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="G93" s="2">
         <v>92</v>
@@ -20346,10 +20356,10 @@
         <v>84</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F94" s="66" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="G94" s="2">
         <v>93</v>
@@ -20370,10 +20380,10 @@
         <v>84</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F95" s="66" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="G95" s="2">
         <v>94</v>
@@ -20391,13 +20401,13 @@
         <v>Project is Referred to Minister for Process Planning - s.18(1)(b)</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E96" s="55" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="G96" s="2">
         <v>95</v>
@@ -20418,10 +20428,10 @@
         <v>98</v>
       </c>
       <c r="E97" s="55" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="G97" s="2">
         <v>96</v>
@@ -20442,10 +20452,10 @@
         <v>98</v>
       </c>
       <c r="E98" s="55" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G98" s="2">
         <v>97</v>
@@ -20463,13 +20473,13 @@
         <v>Other form of Federal Involvement (Coordination, etc.)</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E99" s="55" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="G99" s="2">
         <v>98</v>
@@ -20490,10 +20500,10 @@
         <v>95</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G100" s="2">
         <v>99</v>
@@ -20517,7 +20527,7 @@
         <v>90</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G101" s="2">
         <v>100</v>
@@ -20541,7 +20551,7 @@
         <v>89</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G102" s="2">
         <v>101</v>
@@ -20565,7 +20575,7 @@
         <v>96</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G103" s="2">
         <v>102</v>
@@ -20586,10 +20596,10 @@
         <v>93</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G104" s="2">
         <v>103</v>
@@ -20613,7 +20623,7 @@
         <v>90</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G105" s="2">
         <v>104</v>
@@ -20637,7 +20647,7 @@
         <v>89</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G106" s="2">
         <v>105</v>
@@ -20661,7 +20671,7 @@
         <v>92</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G107" s="2">
         <v>106</v>
@@ -20682,10 +20692,10 @@
         <v>93</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G108" s="2">
         <v>107</v>
@@ -20706,10 +20716,10 @@
         <v>84</v>
       </c>
       <c r="E109" s="66" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F109" s="66" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G109" s="2">
         <v>108</v>
@@ -20727,13 +20737,13 @@
         <v>EAO's Viewpoint is POSITIVE</v>
       </c>
       <c r="D110" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E110" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="E110" s="1" t="s">
-        <v>297</v>
-      </c>
       <c r="F110" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="G110" s="2">
         <v>109</v>
@@ -20751,13 +20761,13 @@
         <v>EAO's Viewpoint is NEGATIVE</v>
       </c>
       <c r="D111" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E111" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="E111" s="1" t="s">
-        <v>297</v>
-      </c>
       <c r="F111" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="G111" s="2">
         <v>110</v>
@@ -20778,10 +20788,10 @@
         <v>95</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G112" s="2">
         <v>111</v>
@@ -20805,7 +20815,7 @@
         <v>90</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G113" s="2">
         <v>112</v>
@@ -20829,7 +20839,7 @@
         <v>89</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G114" s="2">
         <v>113</v>
@@ -20853,7 +20863,7 @@
         <v>96</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G115" s="2">
         <v>114</v>
@@ -20874,10 +20884,10 @@
         <v>93</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G116" s="2">
         <v>115</v>
@@ -20901,7 +20911,7 @@
         <v>90</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G117" s="2">
         <v>116</v>
@@ -20925,7 +20935,7 @@
         <v>89</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G118" s="2">
         <v>117</v>
@@ -20949,7 +20959,7 @@
         <v>92</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G119" s="2">
         <v>118</v>
@@ -20970,10 +20980,10 @@
         <v>93</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G120" s="2">
         <v>119</v>
@@ -20994,10 +21004,10 @@
         <v>95</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G121" s="2">
         <v>120</v>
@@ -21021,7 +21031,7 @@
         <v>90</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G122" s="2">
         <v>121</v>
@@ -21045,7 +21055,7 @@
         <v>89</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G123" s="2">
         <v>122</v>
@@ -21069,7 +21079,7 @@
         <v>96</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G124" s="2">
         <v>123</v>
@@ -21090,10 +21100,10 @@
         <v>93</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G125" s="2">
         <v>124</v>
@@ -21117,7 +21127,7 @@
         <v>90</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G126" s="2">
         <v>125</v>
@@ -21141,7 +21151,7 @@
         <v>89</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G127" s="2">
         <v>126</v>
@@ -21165,7 +21175,7 @@
         <v>92</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G128" s="2">
         <v>127</v>
@@ -21186,10 +21196,10 @@
         <v>93</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G129" s="2">
         <v>128</v>
@@ -21210,10 +21220,10 @@
         <v>84</v>
       </c>
       <c r="E130" s="66" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F130" s="66" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="G130" s="2">
         <v>129</v>
@@ -21231,13 +21241,13 @@
         <v>EAO's Viewpoint is POSITIVE</v>
       </c>
       <c r="D131" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E131" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="E131" s="1" t="s">
-        <v>297</v>
-      </c>
       <c r="F131" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="G131" s="2">
         <v>130</v>
@@ -21255,13 +21265,13 @@
         <v>EAO's Viewpoint is NEGATIVE</v>
       </c>
       <c r="D132" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E132" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="E132" s="1" t="s">
-        <v>297</v>
-      </c>
       <c r="F132" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="G132" s="2">
         <v>131</v>
@@ -21282,10 +21292,10 @@
         <v>95</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G133" s="2">
         <v>132</v>
@@ -21309,7 +21319,7 @@
         <v>90</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G134" s="2">
         <v>133</v>
@@ -21333,7 +21343,7 @@
         <v>89</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G135" s="2">
         <v>134</v>
@@ -21357,7 +21367,7 @@
         <v>96</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G136" s="2">
         <v>135</v>
@@ -21378,10 +21388,10 @@
         <v>93</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G137" s="2">
         <v>136</v>
@@ -21405,7 +21415,7 @@
         <v>90</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G138" s="2">
         <v>137</v>
@@ -21429,7 +21439,7 @@
         <v>89</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G139" s="2">
         <v>138</v>
@@ -21453,7 +21463,7 @@
         <v>92</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G140" s="2">
         <v>139</v>
@@ -21474,10 +21484,10 @@
         <v>93</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G141" s="2">
         <v>140</v>
@@ -21498,10 +21508,10 @@
         <v>84</v>
       </c>
       <c r="E142" s="66" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F142" s="66" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="G142" s="2">
         <v>141</v>
@@ -21522,10 +21532,10 @@
         <v>85</v>
       </c>
       <c r="E143" s="68" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="G143" s="2">
         <v>142</v>
@@ -21546,10 +21556,10 @@
         <v>88</v>
       </c>
       <c r="E144" s="66" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="G144" s="2">
         <v>143</v>
@@ -21570,10 +21580,10 @@
         <v>95</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G145" s="2">
         <v>144</v>
@@ -21597,7 +21607,7 @@
         <v>90</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G146" s="2">
         <v>145</v>
@@ -21621,7 +21631,7 @@
         <v>89</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G147" s="2">
         <v>146</v>
@@ -21645,7 +21655,7 @@
         <v>96</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G148" s="2">
         <v>147</v>
@@ -21666,10 +21676,10 @@
         <v>93</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G149" s="2">
         <v>148</v>
@@ -21693,7 +21703,7 @@
         <v>90</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G150" s="2">
         <v>149</v>
@@ -21717,7 +21727,7 @@
         <v>89</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G151" s="2">
         <v>150</v>
@@ -21741,7 +21751,7 @@
         <v>92</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G152" s="2">
         <v>151</v>
@@ -21762,10 +21772,10 @@
         <v>93</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G153" s="2">
         <v>152</v>
@@ -21786,10 +21796,10 @@
         <v>84</v>
       </c>
       <c r="E154" s="66" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F154" s="66" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="G154" s="2">
         <v>153</v>
@@ -21813,7 +21823,7 @@
         <v>90</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G155" s="2">
         <v>154</v>
@@ -21837,7 +21847,7 @@
         <v>89</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G156" s="2">
         <v>155</v>
@@ -21861,7 +21871,7 @@
         <v>92</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G157" s="2">
         <v>156</v>
@@ -21882,10 +21892,10 @@
         <v>93</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G158" s="2">
         <v>157</v>
@@ -21906,10 +21916,10 @@
         <v>91</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G159" s="2">
         <v>158</v>
@@ -21930,10 +21940,10 @@
         <v>99</v>
       </c>
       <c r="E160" s="55" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="G160" s="2">
         <v>159</v>
@@ -21954,10 +21964,10 @@
         <v>91</v>
       </c>
       <c r="E161" s="9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G161" s="2">
         <v>160</v>
@@ -21978,10 +21988,10 @@
         <v>93</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G162" s="2">
         <v>161</v>
@@ -23000,27 +23010,13 @@
       <c r="G254" s="2"/>
     </row>
     <row r="257" spans="1:7">
-      <c r="A257" s="52" t="s">
-        <v>295</v>
-      </c>
-      <c r="B257" s="52" t="s">
-        <v>295</v>
-      </c>
-      <c r="C257" s="52" t="s">
-        <v>295</v>
-      </c>
-      <c r="D257" s="52" t="s">
-        <v>295</v>
-      </c>
-      <c r="E257" s="52" t="s">
-        <v>295</v>
-      </c>
-      <c r="F257" s="52" t="s">
-        <v>295</v>
-      </c>
-      <c r="G257" s="52" t="s">
-        <v>295</v>
-      </c>
+      <c r="A257" s="52"/>
+      <c r="B257" s="52"/>
+      <c r="C257" s="52"/>
+      <c r="D257" s="52"/>
+      <c r="E257" s="52"/>
+      <c r="F257" s="52"/>
+      <c r="G257" s="52"/>
     </row>
   </sheetData>
   <autoFilter ref="D1:D257" xr:uid="{00000000-0001-0000-0400-000000000000}"/>
@@ -23269,7 +23265,7 @@
     </row>
     <row r="6" spans="1:59">
       <c r="B6" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>24</v>
@@ -23455,7 +23451,7 @@
       </c>
       <c r="M16" s="8"/>
       <c r="U16" s="55" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="17" spans="8:21">

</xml_diff>

<commit_message>
change phase end event action fix
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/assessment/002_EAC_Assessment.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/assessment/002_EAC_Assessment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\epic\track\code\epictrack-api\src\api\templates\event_templates\assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D598A7FB-D144-4454-9B35-0D4BD8F73DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0891B01-B3C5-4230-8118-3AB25E6D708C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2471" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2471" uniqueCount="393">
   <si>
     <t>No</t>
   </si>
@@ -1085,9 +1085,6 @@
   </si>
   <si>
     <t>[{"phase_name":"Early Engagement","work_type_id": 6, "ea_act_id": 3, "is_active": false }]</t>
-  </si>
-  <si>
-    <t>{"phase_name":"DPD Development (Proponent Time)","work_type_id": 6, "ea_act_id": 3, "event_name": "Start of DPD Development (Day after SoE)", "start_at": 1 }</t>
   </si>
   <si>
     <t>{"phase_name":"Pre-EA (EAC Assessment)","work_type_id": 6, "ea_act_id": 3, "event_name": "Last Day of Pre-EA (EAC Assessment)", "start_at": 28 }</t>
@@ -2140,7 +2137,7 @@
         <v>303</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>9</v>
@@ -2169,7 +2166,7 @@
         <v>152</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>9</v>
@@ -2198,7 +2195,7 @@
         <v>153</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>9</v>
@@ -2227,7 +2224,7 @@
         <v>154</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>9</v>
@@ -2256,7 +2253,7 @@
         <v>155</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>9</v>
@@ -2285,7 +2282,7 @@
         <v>156</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>9</v>
@@ -2314,7 +2311,7 @@
         <v>157</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>9</v>
@@ -2343,7 +2340,7 @@
         <v>158</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>9</v>
@@ -2372,7 +2369,7 @@
         <v>159</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>9</v>
@@ -2401,7 +2398,7 @@
         <v>160</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>9</v>
@@ -2430,7 +2427,7 @@
         <v>161</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>9</v>
@@ -2459,7 +2456,7 @@
         <v>162</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>9</v>
@@ -3109,13 +3106,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:M337"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomRight" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -3173,7 +3171,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" hidden="1">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3212,7 +3210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" hidden="1">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3251,7 +3249,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" hidden="1">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3290,7 +3288,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" hidden="1">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3332,7 +3330,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" hidden="1">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3371,7 +3369,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" hidden="1">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3410,7 +3408,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" hidden="1">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3452,7 +3450,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" hidden="1">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3491,7 +3489,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" hidden="1">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -3530,7 +3528,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" hidden="1">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -3572,7 +3570,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" hidden="1">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -3614,7 +3612,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" hidden="1">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -3653,7 +3651,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" hidden="1">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -3695,7 +3693,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" hidden="1">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -3734,7 +3732,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15" thickBot="1">
+    <row r="16" spans="1:13" hidden="1">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -3773,7 +3771,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15" thickBot="1">
+    <row r="17" spans="1:13" ht="15" hidden="1" thickBot="1">
       <c r="A17" s="2">
         <v>9999</v>
       </c>
@@ -3781,7 +3779,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="63" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E17" s="64" t="s">
         <v>303</v>
@@ -3811,7 +3809,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" hidden="1">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -3850,7 +3848,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" hidden="1">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -3892,7 +3890,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" hidden="1">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -4051,7 +4049,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" hidden="1">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -4093,7 +4091,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" hidden="1">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -4135,7 +4133,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" hidden="1">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -4177,7 +4175,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" hidden="1">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -4258,7 +4256,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" hidden="1">
       <c r="A29" s="2">
         <v>27</v>
       </c>
@@ -4339,7 +4337,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" hidden="1">
       <c r="A31" s="2">
         <v>29</v>
       </c>
@@ -4459,7 +4457,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" hidden="1">
       <c r="A34" s="2">
         <v>32</v>
       </c>
@@ -4579,7 +4577,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" hidden="1">
       <c r="A37" s="2">
         <v>35</v>
       </c>
@@ -4660,7 +4658,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" hidden="1">
       <c r="A39" s="2">
         <v>37</v>
       </c>
@@ -4741,7 +4739,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" hidden="1">
       <c r="A41" s="2">
         <v>39</v>
       </c>
@@ -4783,7 +4781,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" hidden="1">
       <c r="A42" s="2">
         <v>40</v>
       </c>
@@ -4864,7 +4862,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" hidden="1">
       <c r="A44" s="2">
         <v>42</v>
       </c>
@@ -4906,7 +4904,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" hidden="1">
       <c r="A45" s="2">
         <v>43</v>
       </c>
@@ -4948,7 +4946,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" hidden="1">
       <c r="A46" s="2">
         <v>44</v>
       </c>
@@ -4990,7 +4988,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" hidden="1">
       <c r="A47" s="2">
         <v>45</v>
       </c>
@@ -5149,7 +5147,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" hidden="1">
       <c r="A51" s="2">
         <v>49</v>
       </c>
@@ -5191,7 +5189,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" hidden="1">
       <c r="A52" s="2">
         <v>50</v>
       </c>
@@ -5272,7 +5270,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" hidden="1">
       <c r="A54" s="2">
         <v>52</v>
       </c>
@@ -5314,7 +5312,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" hidden="1">
       <c r="A55" s="2">
         <v>53</v>
       </c>
@@ -5395,7 +5393,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" hidden="1">
       <c r="A57" s="2">
         <v>55</v>
       </c>
@@ -5437,7 +5435,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" hidden="1">
       <c r="A58" s="2">
         <v>56</v>
       </c>
@@ -5518,7 +5516,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" hidden="1">
       <c r="A60" s="2">
         <v>58</v>
       </c>
@@ -5560,7 +5558,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" hidden="1">
       <c r="A61" s="2">
         <v>59</v>
       </c>
@@ -5641,7 +5639,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" hidden="1">
       <c r="A63" s="2">
         <v>61</v>
       </c>
@@ -5683,7 +5681,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:13" hidden="1">
       <c r="A64" s="2">
         <v>62</v>
       </c>
@@ -5764,7 +5762,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:13" hidden="1">
       <c r="A66" s="2">
         <v>64</v>
       </c>
@@ -5806,7 +5804,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:13">
+    <row r="67" spans="1:13" hidden="1">
       <c r="A67" s="2">
         <v>65</v>
       </c>
@@ -5926,7 +5924,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:13">
+    <row r="70" spans="1:13" hidden="1">
       <c r="A70" s="2">
         <v>68</v>
       </c>
@@ -5968,7 +5966,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:13">
+    <row r="71" spans="1:13" hidden="1">
       <c r="A71" s="2">
         <v>69</v>
       </c>
@@ -6010,7 +6008,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:13">
+    <row r="72" spans="1:13" hidden="1">
       <c r="A72" s="2">
         <v>70</v>
       </c>
@@ -6049,7 +6047,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:13">
+    <row r="73" spans="1:13" hidden="1">
       <c r="A73" s="2">
         <v>71</v>
       </c>
@@ -6088,7 +6086,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:13">
+    <row r="74" spans="1:13" hidden="1">
       <c r="A74" s="2">
         <v>72</v>
       </c>
@@ -6130,7 +6128,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:13">
+    <row r="75" spans="1:13" hidden="1">
       <c r="A75" s="2">
         <v>73</v>
       </c>
@@ -6169,7 +6167,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:13">
+    <row r="76" spans="1:13" hidden="1">
       <c r="A76" s="2">
         <v>74</v>
       </c>
@@ -6208,7 +6206,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:13">
+    <row r="77" spans="1:13" hidden="1">
       <c r="A77" s="2">
         <v>75</v>
       </c>
@@ -6250,7 +6248,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:13">
+    <row r="78" spans="1:13" hidden="1">
       <c r="A78" s="2">
         <v>76</v>
       </c>
@@ -6289,7 +6287,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:13">
+    <row r="79" spans="1:13" hidden="1">
       <c r="A79" s="2">
         <v>77</v>
       </c>
@@ -6331,7 +6329,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:13">
+    <row r="80" spans="1:13" hidden="1">
       <c r="A80" s="2">
         <v>78</v>
       </c>
@@ -6373,7 +6371,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:13">
+    <row r="81" spans="1:13" hidden="1">
       <c r="A81" s="2">
         <v>79</v>
       </c>
@@ -6412,7 +6410,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:13">
+    <row r="82" spans="1:13" hidden="1">
       <c r="A82" s="2">
         <v>80</v>
       </c>
@@ -6454,7 +6452,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:13">
+    <row r="83" spans="1:13" hidden="1">
       <c r="A83" s="2">
         <v>81</v>
       </c>
@@ -6496,7 +6494,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:13">
+    <row r="84" spans="1:13" hidden="1">
       <c r="A84" s="2">
         <v>82</v>
       </c>
@@ -6535,7 +6533,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:13">
+    <row r="85" spans="1:13" hidden="1">
       <c r="A85" s="2">
         <v>83</v>
       </c>
@@ -6577,7 +6575,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:13">
+    <row r="86" spans="1:13" hidden="1">
       <c r="A86" s="2">
         <v>84</v>
       </c>
@@ -6619,7 +6617,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:13">
+    <row r="87" spans="1:13" hidden="1">
       <c r="A87" s="2">
         <v>85</v>
       </c>
@@ -6658,7 +6656,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:13">
+    <row r="88" spans="1:13" hidden="1">
       <c r="A88" s="2">
         <v>86</v>
       </c>
@@ -6697,7 +6695,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:13">
+    <row r="89" spans="1:13" hidden="1">
       <c r="A89" s="2">
         <v>87</v>
       </c>
@@ -6736,7 +6734,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:13">
+    <row r="90" spans="1:13" hidden="1">
       <c r="A90" s="2">
         <v>88</v>
       </c>
@@ -6778,7 +6776,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:13">
+    <row r="91" spans="1:13" hidden="1">
       <c r="A91" s="2">
         <v>89</v>
       </c>
@@ -6820,7 +6818,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:13">
+    <row r="92" spans="1:13" hidden="1">
       <c r="A92" s="2">
         <v>90</v>
       </c>
@@ -6859,7 +6857,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:13">
+    <row r="93" spans="1:13" hidden="1">
       <c r="A93" s="2">
         <v>91</v>
       </c>
@@ -6901,7 +6899,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:13">
+    <row r="94" spans="1:13" hidden="1">
       <c r="A94" s="2">
         <v>92</v>
       </c>
@@ -6940,7 +6938,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:13">
+    <row r="95" spans="1:13" hidden="1">
       <c r="A95" s="2">
         <v>93</v>
       </c>
@@ -6979,7 +6977,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:13">
+    <row r="96" spans="1:13" hidden="1">
       <c r="A96" s="2">
         <v>94</v>
       </c>
@@ -7021,7 +7019,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:13">
+    <row r="97" spans="1:13" hidden="1">
       <c r="A97" s="2">
         <v>95</v>
       </c>
@@ -7060,7 +7058,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:13">
+    <row r="98" spans="1:13" hidden="1">
       <c r="A98" s="2">
         <v>96</v>
       </c>
@@ -7099,7 +7097,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:13">
+    <row r="99" spans="1:13" hidden="1">
       <c r="A99" s="2">
         <v>97</v>
       </c>
@@ -7141,7 +7139,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:13">
+    <row r="100" spans="1:13" hidden="1">
       <c r="A100" s="2">
         <v>98</v>
       </c>
@@ -7183,7 +7181,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:13">
+    <row r="101" spans="1:13" hidden="1">
       <c r="A101" s="2">
         <v>99</v>
       </c>
@@ -7222,7 +7220,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:13">
+    <row r="102" spans="1:13" hidden="1">
       <c r="A102" s="2">
         <v>100</v>
       </c>
@@ -7264,7 +7262,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:13">
+    <row r="103" spans="1:13" hidden="1">
       <c r="A103" s="2">
         <v>101</v>
       </c>
@@ -7306,7 +7304,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:13">
+    <row r="104" spans="1:13" hidden="1">
       <c r="A104" s="2">
         <v>102</v>
       </c>
@@ -7345,7 +7343,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:13">
+    <row r="105" spans="1:13" hidden="1">
       <c r="A105" s="2">
         <v>103</v>
       </c>
@@ -7387,7 +7385,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:13">
+    <row r="106" spans="1:13" hidden="1">
       <c r="A106" s="2">
         <v>104</v>
       </c>
@@ -7429,7 +7427,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:13" ht="15" thickBot="1">
+    <row r="107" spans="1:13" hidden="1">
       <c r="A107" s="2">
         <v>105</v>
       </c>
@@ -7468,7 +7466,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:13">
+    <row r="108" spans="1:13" hidden="1">
       <c r="A108" s="41">
         <v>106</v>
       </c>
@@ -7508,7 +7506,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:13" ht="15" thickBot="1">
+    <row r="109" spans="1:13" ht="15" hidden="1" thickBot="1">
       <c r="A109" s="42">
         <v>107</v>
       </c>
@@ -7548,7 +7546,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:13">
+    <row r="110" spans="1:13" hidden="1">
       <c r="A110" s="2">
         <v>108</v>
       </c>
@@ -7587,7 +7585,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:13">
+    <row r="111" spans="1:13" hidden="1">
       <c r="A111" s="2">
         <v>109</v>
       </c>
@@ -7629,7 +7627,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:13">
+    <row r="112" spans="1:13" hidden="1">
       <c r="A112" s="2">
         <v>110</v>
       </c>
@@ -7671,7 +7669,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="113" spans="1:13">
+    <row r="113" spans="1:13" hidden="1">
       <c r="A113" s="2">
         <v>111</v>
       </c>
@@ -7710,7 +7708,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="114" spans="1:13">
+    <row r="114" spans="1:13" hidden="1">
       <c r="A114" s="2">
         <v>112</v>
       </c>
@@ -7749,7 +7747,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="115" spans="1:13">
+    <row r="115" spans="1:13" hidden="1">
       <c r="A115" s="2">
         <v>113</v>
       </c>
@@ -7788,7 +7786,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="116" spans="1:13">
+    <row r="116" spans="1:13" hidden="1">
       <c r="A116" s="2">
         <v>114</v>
       </c>
@@ -7830,7 +7828,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="117" spans="1:13">
+    <row r="117" spans="1:13" hidden="1">
       <c r="A117" s="2">
         <v>115</v>
       </c>
@@ -7872,7 +7870,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="118" spans="1:13">
+    <row r="118" spans="1:13" hidden="1">
       <c r="A118" s="2">
         <v>116</v>
       </c>
@@ -7911,7 +7909,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="119" spans="1:13">
+    <row r="119" spans="1:13" hidden="1">
       <c r="A119" s="2">
         <v>117</v>
       </c>
@@ -7953,7 +7951,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="120" spans="1:13">
+    <row r="120" spans="1:13" hidden="1">
       <c r="A120" s="2">
         <v>118</v>
       </c>
@@ -7995,7 +7993,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="121" spans="1:13">
+    <row r="121" spans="1:13" hidden="1">
       <c r="A121" s="2">
         <v>119</v>
       </c>
@@ -8034,7 +8032,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="122" spans="1:13">
+    <row r="122" spans="1:13" hidden="1">
       <c r="A122" s="2">
         <v>120</v>
       </c>
@@ -8073,7 +8071,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="123" spans="1:13">
+    <row r="123" spans="1:13" hidden="1">
       <c r="A123" s="2">
         <v>121</v>
       </c>
@@ -8115,7 +8113,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="124" spans="1:13">
+    <row r="124" spans="1:13" hidden="1">
       <c r="A124" s="2">
         <v>122</v>
       </c>
@@ -8154,7 +8152,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="125" spans="1:13">
+    <row r="125" spans="1:13" hidden="1">
       <c r="A125" s="2">
         <v>123</v>
       </c>
@@ -8193,7 +8191,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="126" spans="1:13">
+    <row r="126" spans="1:13" hidden="1">
       <c r="A126" s="2">
         <v>124</v>
       </c>
@@ -8232,7 +8230,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="127" spans="1:13">
+    <row r="127" spans="1:13" hidden="1">
       <c r="A127" s="2">
         <v>125</v>
       </c>
@@ -8271,7 +8269,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="128" spans="1:13">
+    <row r="128" spans="1:13" hidden="1">
       <c r="A128" s="2">
         <v>126</v>
       </c>
@@ -8310,7 +8308,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="129" spans="1:13">
+    <row r="129" spans="1:13" hidden="1">
       <c r="A129" s="2">
         <v>127</v>
       </c>
@@ -8349,7 +8347,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="130" spans="1:13">
+    <row r="130" spans="1:13" hidden="1">
       <c r="A130" s="2">
         <v>128</v>
       </c>
@@ -8388,7 +8386,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="131" spans="1:13">
+    <row r="131" spans="1:13" hidden="1">
       <c r="A131" s="2">
         <v>129</v>
       </c>
@@ -8427,7 +8425,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="132" spans="1:13" ht="15" thickBot="1">
+    <row r="132" spans="1:13" hidden="1">
       <c r="A132" s="2">
         <v>130</v>
       </c>
@@ -8466,7 +8464,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="133" spans="1:13" ht="15" thickBot="1">
+    <row r="133" spans="1:13" ht="15" hidden="1" thickBot="1">
       <c r="A133" s="44">
         <v>131</v>
       </c>
@@ -8504,7 +8502,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="134" spans="1:13">
+    <row r="134" spans="1:13" hidden="1">
       <c r="A134" s="2">
         <v>132</v>
       </c>
@@ -8543,7 +8541,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="135" spans="1:13">
+    <row r="135" spans="1:13" hidden="1">
       <c r="A135" s="2">
         <v>133</v>
       </c>
@@ -8585,7 +8583,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="136" spans="1:13">
+    <row r="136" spans="1:13" hidden="1">
       <c r="A136" s="2">
         <v>134</v>
       </c>
@@ -8627,7 +8625,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="137" spans="1:13">
+    <row r="137" spans="1:13" hidden="1">
       <c r="A137" s="2">
         <v>135</v>
       </c>
@@ -8666,7 +8664,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="138" spans="1:13">
+    <row r="138" spans="1:13" hidden="1">
       <c r="A138" s="2">
         <v>136</v>
       </c>
@@ -8705,7 +8703,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="139" spans="1:13">
+    <row r="139" spans="1:13" hidden="1">
       <c r="A139" s="2">
         <v>137</v>
       </c>
@@ -8747,7 +8745,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="140" spans="1:13">
+    <row r="140" spans="1:13" hidden="1">
       <c r="A140" s="2">
         <v>138</v>
       </c>
@@ -8789,7 +8787,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="141" spans="1:13">
+    <row r="141" spans="1:13" hidden="1">
       <c r="A141" s="2">
         <v>139</v>
       </c>
@@ -8828,7 +8826,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="142" spans="1:13">
+    <row r="142" spans="1:13" hidden="1">
       <c r="A142" s="2">
         <v>140</v>
       </c>
@@ -8867,7 +8865,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="143" spans="1:13">
+    <row r="143" spans="1:13" hidden="1">
       <c r="A143" s="2">
         <v>141</v>
       </c>
@@ -8909,7 +8907,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="144" spans="1:13">
+    <row r="144" spans="1:13" hidden="1">
       <c r="A144" s="2">
         <v>142</v>
       </c>
@@ -8951,7 +8949,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="145" spans="1:13">
+    <row r="145" spans="1:13" hidden="1">
       <c r="A145" s="2">
         <v>143</v>
       </c>
@@ -8993,7 +8991,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="146" spans="1:13">
+    <row r="146" spans="1:13" hidden="1">
       <c r="A146" s="2">
         <v>144</v>
       </c>
@@ -9035,7 +9033,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="147" spans="1:13">
+    <row r="147" spans="1:13" hidden="1">
       <c r="A147" s="2">
         <v>145</v>
       </c>
@@ -9074,7 +9072,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="148" spans="1:13">
+    <row r="148" spans="1:13" hidden="1">
       <c r="A148" s="2">
         <v>146</v>
       </c>
@@ -9113,7 +9111,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="149" spans="1:13">
+    <row r="149" spans="1:13" hidden="1">
       <c r="A149" s="2">
         <v>147</v>
       </c>
@@ -9155,7 +9153,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="150" spans="1:13">
+    <row r="150" spans="1:13" hidden="1">
       <c r="A150" s="2">
         <v>148</v>
       </c>
@@ -9194,7 +9192,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="151" spans="1:13">
+    <row r="151" spans="1:13" hidden="1">
       <c r="A151" s="2">
         <v>149</v>
       </c>
@@ -9233,7 +9231,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="152" spans="1:13">
+    <row r="152" spans="1:13" hidden="1">
       <c r="A152" s="2">
         <v>150</v>
       </c>
@@ -9272,7 +9270,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="153" spans="1:13">
+    <row r="153" spans="1:13" hidden="1">
       <c r="A153" s="2">
         <v>151</v>
       </c>
@@ -9311,7 +9309,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="154" spans="1:13">
+    <row r="154" spans="1:13" hidden="1">
       <c r="A154" s="2">
         <v>152</v>
       </c>
@@ -9350,7 +9348,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="155" spans="1:13">
+    <row r="155" spans="1:13" hidden="1">
       <c r="A155" s="2">
         <v>153</v>
       </c>
@@ -9392,7 +9390,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="156" spans="1:13">
+    <row r="156" spans="1:13" hidden="1">
       <c r="A156" s="2">
         <v>154</v>
       </c>
@@ -9434,7 +9432,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="157" spans="1:13">
+    <row r="157" spans="1:13" hidden="1">
       <c r="A157" s="2">
         <v>155</v>
       </c>
@@ -9473,7 +9471,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="158" spans="1:13">
+    <row r="158" spans="1:13" hidden="1">
       <c r="A158" s="2">
         <v>156</v>
       </c>
@@ -9515,7 +9513,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="159" spans="1:13">
+    <row r="159" spans="1:13" hidden="1">
       <c r="A159" s="2">
         <v>157</v>
       </c>
@@ -9557,7 +9555,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="160" spans="1:13">
+    <row r="160" spans="1:13" hidden="1">
       <c r="A160" s="2">
         <v>158</v>
       </c>
@@ -9599,7 +9597,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="161" spans="1:13">
+    <row r="161" spans="1:13" hidden="1">
       <c r="A161" s="2">
         <v>159</v>
       </c>
@@ -9641,7 +9639,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="162" spans="1:13">
+    <row r="162" spans="1:13" hidden="1">
       <c r="A162" s="2">
         <v>160</v>
       </c>
@@ -9680,7 +9678,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="163" spans="1:13">
+    <row r="163" spans="1:13" hidden="1">
       <c r="A163" s="2">
         <v>161</v>
       </c>
@@ -9719,7 +9717,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="164" spans="1:13">
+    <row r="164" spans="1:13" hidden="1">
       <c r="A164" s="2">
         <v>162</v>
       </c>
@@ -9758,7 +9756,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="165" spans="1:13">
+    <row r="165" spans="1:13" hidden="1">
       <c r="A165" s="2">
         <v>163</v>
       </c>
@@ -9800,7 +9798,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="166" spans="1:13">
+    <row r="166" spans="1:13" hidden="1">
       <c r="A166" s="2">
         <v>164</v>
       </c>
@@ -9842,7 +9840,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="167" spans="1:13">
+    <row r="167" spans="1:13" hidden="1">
       <c r="A167" s="2">
         <v>165</v>
       </c>
@@ -9881,7 +9879,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="168" spans="1:13">
+    <row r="168" spans="1:13" hidden="1">
       <c r="A168" s="2">
         <v>166</v>
       </c>
@@ -9923,7 +9921,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="169" spans="1:13">
+    <row r="169" spans="1:13" hidden="1">
       <c r="A169" s="2">
         <v>167</v>
       </c>
@@ -9965,7 +9963,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="170" spans="1:13">
+    <row r="170" spans="1:13" hidden="1">
       <c r="A170" s="2">
         <v>168</v>
       </c>
@@ -10004,7 +10002,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="171" spans="1:13">
+    <row r="171" spans="1:13" hidden="1">
       <c r="A171" s="2">
         <v>169</v>
       </c>
@@ -10046,7 +10044,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="172" spans="1:13">
+    <row r="172" spans="1:13" hidden="1">
       <c r="A172" s="2">
         <v>170</v>
       </c>
@@ -10088,7 +10086,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="173" spans="1:13">
+    <row r="173" spans="1:13" hidden="1">
       <c r="A173" s="2">
         <v>171</v>
       </c>
@@ -10127,7 +10125,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="174" spans="1:13">
+    <row r="174" spans="1:13" hidden="1">
       <c r="A174" s="2">
         <v>172</v>
       </c>
@@ -10169,7 +10167,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="175" spans="1:13">
+    <row r="175" spans="1:13" hidden="1">
       <c r="A175" s="2">
         <v>173</v>
       </c>
@@ -10211,7 +10209,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="176" spans="1:13">
+    <row r="176" spans="1:13" hidden="1">
       <c r="A176" s="2">
         <v>174</v>
       </c>
@@ -10250,7 +10248,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="177" spans="1:13">
+    <row r="177" spans="1:13" hidden="1">
       <c r="A177" s="2">
         <v>175</v>
       </c>
@@ -10292,7 +10290,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="178" spans="1:13">
+    <row r="178" spans="1:13" hidden="1">
       <c r="A178" s="2">
         <v>176</v>
       </c>
@@ -10334,7 +10332,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="179" spans="1:13">
+    <row r="179" spans="1:13" hidden="1">
       <c r="A179" s="2">
         <v>177</v>
       </c>
@@ -10373,7 +10371,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="180" spans="1:13">
+    <row r="180" spans="1:13" hidden="1">
       <c r="A180" s="2">
         <v>178</v>
       </c>
@@ -10415,7 +10413,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="181" spans="1:13">
+    <row r="181" spans="1:13" hidden="1">
       <c r="A181" s="2">
         <v>179</v>
       </c>
@@ -10457,7 +10455,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="182" spans="1:13">
+    <row r="182" spans="1:13" hidden="1">
       <c r="A182" s="2">
         <v>180</v>
       </c>
@@ -10496,7 +10494,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="183" spans="1:13">
+    <row r="183" spans="1:13" hidden="1">
       <c r="A183" s="2">
         <v>181</v>
       </c>
@@ -10535,7 +10533,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="184" spans="1:13">
+    <row r="184" spans="1:13" hidden="1">
       <c r="A184" s="2">
         <v>182</v>
       </c>
@@ -10577,7 +10575,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="185" spans="1:13">
+    <row r="185" spans="1:13" hidden="1">
       <c r="A185" s="2">
         <v>183</v>
       </c>
@@ -10619,7 +10617,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="186" spans="1:13">
+    <row r="186" spans="1:13" hidden="1">
       <c r="A186" s="2">
         <v>184</v>
       </c>
@@ -10658,7 +10656,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="187" spans="1:13">
+    <row r="187" spans="1:13" hidden="1">
       <c r="A187" s="2">
         <v>185</v>
       </c>
@@ -10697,7 +10695,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="188" spans="1:13">
+    <row r="188" spans="1:13" hidden="1">
       <c r="A188" s="2">
         <v>186</v>
       </c>
@@ -10739,7 +10737,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="189" spans="1:13">
+    <row r="189" spans="1:13" hidden="1">
       <c r="A189" s="2">
         <v>187</v>
       </c>
@@ -10778,7 +10776,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="190" spans="1:13">
+    <row r="190" spans="1:13" hidden="1">
       <c r="A190" s="2">
         <v>188</v>
       </c>
@@ -10817,7 +10815,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="191" spans="1:13">
+    <row r="191" spans="1:13" hidden="1">
       <c r="A191" s="2">
         <v>189</v>
       </c>
@@ -10859,7 +10857,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="192" spans="1:13">
+    <row r="192" spans="1:13" hidden="1">
       <c r="A192" s="2">
         <v>190</v>
       </c>
@@ -10898,7 +10896,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="193" spans="1:13">
+    <row r="193" spans="1:13" hidden="1">
       <c r="A193" s="2">
         <v>191</v>
       </c>
@@ -10940,7 +10938,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="194" spans="1:13">
+    <row r="194" spans="1:13" hidden="1">
       <c r="A194" s="2">
         <v>192</v>
       </c>
@@ -10979,7 +10977,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="195" spans="1:13">
+    <row r="195" spans="1:13" hidden="1">
       <c r="A195" s="2">
         <v>193</v>
       </c>
@@ -11021,7 +11019,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="196" spans="1:13">
+    <row r="196" spans="1:13" hidden="1">
       <c r="A196" s="2">
         <v>194</v>
       </c>
@@ -11063,7 +11061,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="197" spans="1:13">
+    <row r="197" spans="1:13" hidden="1">
       <c r="A197" s="2">
         <v>195</v>
       </c>
@@ -11102,7 +11100,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="198" spans="1:13">
+    <row r="198" spans="1:13" hidden="1">
       <c r="A198" s="2">
         <v>196</v>
       </c>
@@ -11144,7 +11142,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="199" spans="1:13">
+    <row r="199" spans="1:13" hidden="1">
       <c r="A199" s="2">
         <v>197</v>
       </c>
@@ -11186,7 +11184,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="200" spans="1:13">
+    <row r="200" spans="1:13" hidden="1">
       <c r="A200" s="2">
         <v>198</v>
       </c>
@@ -11225,7 +11223,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="201" spans="1:13">
+    <row r="201" spans="1:13" hidden="1">
       <c r="A201" s="2">
         <v>199</v>
       </c>
@@ -11267,7 +11265,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="202" spans="1:13">
+    <row r="202" spans="1:13" hidden="1">
       <c r="A202" s="2">
         <v>200</v>
       </c>
@@ -11309,7 +11307,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="203" spans="1:13">
+    <row r="203" spans="1:13" hidden="1">
       <c r="A203" s="2">
         <v>201</v>
       </c>
@@ -11348,7 +11346,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="204" spans="1:13">
+    <row r="204" spans="1:13" hidden="1">
       <c r="A204" s="2">
         <v>202</v>
       </c>
@@ -11387,7 +11385,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="205" spans="1:13">
+    <row r="205" spans="1:13" hidden="1">
       <c r="A205" s="2">
         <v>203</v>
       </c>
@@ -11426,7 +11424,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="206" spans="1:13">
+    <row r="206" spans="1:13" hidden="1">
       <c r="A206" s="2">
         <v>204</v>
       </c>
@@ -11468,7 +11466,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="207" spans="1:13">
+    <row r="207" spans="1:13" hidden="1">
       <c r="A207" s="2">
         <v>205</v>
       </c>
@@ -11510,7 +11508,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="208" spans="1:13">
+    <row r="208" spans="1:13" hidden="1">
       <c r="A208" s="2">
         <v>206</v>
       </c>
@@ -11549,7 +11547,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="209" spans="1:13">
+    <row r="209" spans="1:13" hidden="1">
       <c r="A209" s="2">
         <v>207</v>
       </c>
@@ -11591,7 +11589,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="210" spans="1:13">
+    <row r="210" spans="1:13" hidden="1">
       <c r="A210" s="2">
         <v>208</v>
       </c>
@@ -11633,7 +11631,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="211" spans="1:13">
+    <row r="211" spans="1:13" hidden="1">
       <c r="A211" s="2">
         <v>209</v>
       </c>
@@ -11675,7 +11673,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="212" spans="1:13">
+    <row r="212" spans="1:13" hidden="1">
       <c r="A212" s="2">
         <v>210</v>
       </c>
@@ -11717,7 +11715,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="213" spans="1:13">
+    <row r="213" spans="1:13" hidden="1">
       <c r="A213" s="2">
         <v>211</v>
       </c>
@@ -11756,7 +11754,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="214" spans="1:13">
+    <row r="214" spans="1:13" hidden="1">
       <c r="A214" s="2">
         <v>212</v>
       </c>
@@ -11798,7 +11796,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="215" spans="1:13">
+    <row r="215" spans="1:13" hidden="1">
       <c r="A215" s="2">
         <v>213</v>
       </c>
@@ -11837,7 +11835,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="216" spans="1:13">
+    <row r="216" spans="1:13" hidden="1">
       <c r="A216" s="2">
         <v>214</v>
       </c>
@@ -11879,7 +11877,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="217" spans="1:13">
+    <row r="217" spans="1:13" hidden="1">
       <c r="A217" s="2">
         <v>215</v>
       </c>
@@ -11918,7 +11916,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="218" spans="1:13">
+    <row r="218" spans="1:13" hidden="1">
       <c r="A218" s="2">
         <v>216</v>
       </c>
@@ -11957,7 +11955,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="219" spans="1:13">
+    <row r="219" spans="1:13" hidden="1">
       <c r="A219" s="2">
         <v>217</v>
       </c>
@@ -11999,7 +11997,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="220" spans="1:13">
+    <row r="220" spans="1:13" hidden="1">
       <c r="A220" s="2">
         <v>218</v>
       </c>
@@ -12038,7 +12036,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="221" spans="1:13">
+    <row r="221" spans="1:13" hidden="1">
       <c r="A221" s="2">
         <v>219</v>
       </c>
@@ -12080,7 +12078,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="222" spans="1:13">
+    <row r="222" spans="1:13" hidden="1">
       <c r="A222" s="2">
         <v>220</v>
       </c>
@@ -12122,7 +12120,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="223" spans="1:13">
+    <row r="223" spans="1:13" hidden="1">
       <c r="A223" s="2">
         <v>221</v>
       </c>
@@ -12161,7 +12159,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="224" spans="1:13">
+    <row r="224" spans="1:13" hidden="1">
       <c r="A224" s="2">
         <v>222</v>
       </c>
@@ -12203,7 +12201,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="225" spans="1:13">
+    <row r="225" spans="1:13" hidden="1">
       <c r="A225" s="2">
         <v>223</v>
       </c>
@@ -12245,7 +12243,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="226" spans="1:13">
+    <row r="226" spans="1:13" hidden="1">
       <c r="A226" s="2">
         <v>224</v>
       </c>
@@ -12287,7 +12285,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="227" spans="1:13">
+    <row r="227" spans="1:13" hidden="1">
       <c r="A227" s="2">
         <v>225</v>
       </c>
@@ -12329,7 +12327,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="228" spans="1:13">
+    <row r="228" spans="1:13" hidden="1">
       <c r="A228" s="2">
         <v>226</v>
       </c>
@@ -12368,7 +12366,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="229" spans="1:13">
+    <row r="229" spans="1:13" hidden="1">
       <c r="A229" s="2">
         <v>227</v>
       </c>
@@ -12407,7 +12405,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="230" spans="1:13">
+    <row r="230" spans="1:13" hidden="1">
       <c r="A230" s="2">
         <v>228</v>
       </c>
@@ -12446,7 +12444,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="231" spans="1:13">
+    <row r="231" spans="1:13" hidden="1">
       <c r="A231" s="2">
         <v>229</v>
       </c>
@@ -12488,7 +12486,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="232" spans="1:13">
+    <row r="232" spans="1:13" hidden="1">
       <c r="A232" s="2">
         <v>230</v>
       </c>
@@ -12530,7 +12528,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="233" spans="1:13">
+    <row r="233" spans="1:13" hidden="1">
       <c r="A233" s="2">
         <v>231</v>
       </c>
@@ -12569,7 +12567,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="234" spans="1:13">
+    <row r="234" spans="1:13" hidden="1">
       <c r="A234" s="2">
         <v>232</v>
       </c>
@@ -12611,7 +12609,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="235" spans="1:13">
+    <row r="235" spans="1:13" hidden="1">
       <c r="A235" s="2">
         <v>233</v>
       </c>
@@ -12653,7 +12651,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="236" spans="1:13">
+    <row r="236" spans="1:13" hidden="1">
       <c r="A236" s="2">
         <v>234</v>
       </c>
@@ -12692,7 +12690,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="237" spans="1:13">
+    <row r="237" spans="1:13" hidden="1">
       <c r="A237" s="2">
         <v>235</v>
       </c>
@@ -12734,7 +12732,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="238" spans="1:13">
+    <row r="238" spans="1:13" hidden="1">
       <c r="A238" s="2">
         <v>236</v>
       </c>
@@ -12776,7 +12774,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="239" spans="1:13">
+    <row r="239" spans="1:13" hidden="1">
       <c r="A239" s="2">
         <v>237</v>
       </c>
@@ -12815,7 +12813,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="240" spans="1:13">
+    <row r="240" spans="1:13" hidden="1">
       <c r="A240" s="2">
         <v>238</v>
       </c>
@@ -12857,7 +12855,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="241" spans="1:13">
+    <row r="241" spans="1:13" hidden="1">
       <c r="A241" s="2">
         <v>239</v>
       </c>
@@ -12899,7 +12897,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="242" spans="1:13">
+    <row r="242" spans="1:13" hidden="1">
       <c r="A242" s="2">
         <v>240</v>
       </c>
@@ -12938,7 +12936,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="243" spans="1:13">
+    <row r="243" spans="1:13" hidden="1">
       <c r="A243" s="2">
         <v>241</v>
       </c>
@@ -12980,7 +12978,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="244" spans="1:13">
+    <row r="244" spans="1:13" hidden="1">
       <c r="A244" s="2">
         <v>242</v>
       </c>
@@ -13022,7 +13020,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="245" spans="1:13">
+    <row r="245" spans="1:13" hidden="1">
       <c r="A245" s="2">
         <v>243</v>
       </c>
@@ -13061,7 +13059,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="246" spans="1:13">
+    <row r="246" spans="1:13" hidden="1">
       <c r="A246" s="2">
         <v>244</v>
       </c>
@@ -13103,7 +13101,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="247" spans="1:13">
+    <row r="247" spans="1:13" hidden="1">
       <c r="A247" s="2">
         <v>245</v>
       </c>
@@ -13145,7 +13143,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="248" spans="1:13">
+    <row r="248" spans="1:13" hidden="1">
       <c r="A248" s="2">
         <v>246</v>
       </c>
@@ -13184,7 +13182,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="249" spans="1:13">
+    <row r="249" spans="1:13" hidden="1">
       <c r="A249" s="2">
         <v>247</v>
       </c>
@@ -13223,7 +13221,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="250" spans="1:13">
+    <row r="250" spans="1:13" hidden="1">
       <c r="A250" s="2">
         <v>248</v>
       </c>
@@ -13265,7 +13263,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="251" spans="1:13">
+    <row r="251" spans="1:13" hidden="1">
       <c r="A251" s="2">
         <v>249</v>
       </c>
@@ -13307,7 +13305,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="252" spans="1:13">
+    <row r="252" spans="1:13" hidden="1">
       <c r="A252" s="2">
         <v>250</v>
       </c>
@@ -13346,7 +13344,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="253" spans="1:13">
+    <row r="253" spans="1:13" hidden="1">
       <c r="A253" s="2">
         <v>251</v>
       </c>
@@ -13385,7 +13383,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="254" spans="1:13">
+    <row r="254" spans="1:13" hidden="1">
       <c r="A254" s="2">
         <v>252</v>
       </c>
@@ -13424,7 +13422,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="255" spans="1:13">
+    <row r="255" spans="1:13" hidden="1">
       <c r="A255" s="2">
         <v>253</v>
       </c>
@@ -13466,7 +13464,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="256" spans="1:13">
+    <row r="256" spans="1:13" hidden="1">
       <c r="A256" s="2">
         <v>254</v>
       </c>
@@ -13505,7 +13503,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="257" spans="1:13">
+    <row r="257" spans="1:13" hidden="1">
       <c r="A257" s="2">
         <v>255</v>
       </c>
@@ -13544,7 +13542,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="258" spans="1:13">
+    <row r="258" spans="1:13" hidden="1">
       <c r="A258" s="2">
         <v>256</v>
       </c>
@@ -13586,7 +13584,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="259" spans="1:13">
+    <row r="259" spans="1:13" hidden="1">
       <c r="A259" s="2">
         <v>257</v>
       </c>
@@ -13625,7 +13623,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="260" spans="1:13">
+    <row r="260" spans="1:13" hidden="1">
       <c r="A260" s="2">
         <v>258</v>
       </c>
@@ -13667,7 +13665,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="261" spans="1:13">
+    <row r="261" spans="1:13" hidden="1">
       <c r="A261" s="2">
         <v>259</v>
       </c>
@@ -13706,7 +13704,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="262" spans="1:13">
+    <row r="262" spans="1:13" hidden="1">
       <c r="A262" s="2">
         <v>260</v>
       </c>
@@ -13748,7 +13746,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="263" spans="1:13">
+    <row r="263" spans="1:13" hidden="1">
       <c r="A263" s="2">
         <v>261</v>
       </c>
@@ -13790,7 +13788,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="264" spans="1:13">
+    <row r="264" spans="1:13" hidden="1">
       <c r="A264" s="2">
         <v>262</v>
       </c>
@@ -13829,7 +13827,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="265" spans="1:13">
+    <row r="265" spans="1:13" hidden="1">
       <c r="A265" s="2">
         <v>263</v>
       </c>
@@ -13871,7 +13869,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="266" spans="1:13">
+    <row r="266" spans="1:13" hidden="1">
       <c r="A266" s="2">
         <v>264</v>
       </c>
@@ -13913,7 +13911,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="267" spans="1:13">
+    <row r="267" spans="1:13" hidden="1">
       <c r="A267" s="2">
         <v>265</v>
       </c>
@@ -13952,7 +13950,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="268" spans="1:13">
+    <row r="268" spans="1:13" hidden="1">
       <c r="A268" s="2">
         <v>266</v>
       </c>
@@ -13994,7 +13992,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="269" spans="1:13">
+    <row r="269" spans="1:13" hidden="1">
       <c r="A269" s="2">
         <v>267</v>
       </c>
@@ -14036,7 +14034,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="270" spans="1:13">
+    <row r="270" spans="1:13" hidden="1">
       <c r="A270" s="2">
         <v>268</v>
       </c>
@@ -14075,7 +14073,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="271" spans="1:13">
+    <row r="271" spans="1:13" hidden="1">
       <c r="A271" s="2">
         <v>269</v>
       </c>
@@ -14114,7 +14112,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="272" spans="1:13">
+    <row r="272" spans="1:13" hidden="1">
       <c r="A272" s="2">
         <v>270</v>
       </c>
@@ -14153,7 +14151,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="273" spans="1:13">
+    <row r="273" spans="1:13" hidden="1">
       <c r="A273" s="2">
         <v>271</v>
       </c>
@@ -14192,7 +14190,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="274" spans="1:13">
+    <row r="274" spans="1:13" hidden="1">
       <c r="A274" s="2">
         <v>272</v>
       </c>
@@ -14231,7 +14229,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="275" spans="1:13">
+    <row r="275" spans="1:13" hidden="1">
       <c r="A275" s="2">
         <v>273</v>
       </c>
@@ -14273,7 +14271,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="276" spans="1:13">
+    <row r="276" spans="1:13" hidden="1">
       <c r="A276" s="2">
         <v>274</v>
       </c>
@@ -14315,7 +14313,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="277" spans="1:13">
+    <row r="277" spans="1:13" hidden="1">
       <c r="A277" s="2">
         <v>275</v>
       </c>
@@ -14354,7 +14352,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="278" spans="1:13">
+    <row r="278" spans="1:13" hidden="1">
       <c r="A278" s="2">
         <v>276</v>
       </c>
@@ -14393,7 +14391,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="279" spans="1:13">
+    <row r="279" spans="1:13" hidden="1">
       <c r="A279" s="2">
         <v>277</v>
       </c>
@@ -14435,7 +14433,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="280" spans="1:13">
+    <row r="280" spans="1:13" hidden="1">
       <c r="A280" s="2">
         <v>278</v>
       </c>
@@ -14477,7 +14475,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="281" spans="1:13">
+    <row r="281" spans="1:13" hidden="1">
       <c r="A281" s="2">
         <v>279</v>
       </c>
@@ -14519,7 +14517,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="282" spans="1:13">
+    <row r="282" spans="1:13" hidden="1">
       <c r="A282" s="2">
         <v>280</v>
       </c>
@@ -14561,7 +14559,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="283" spans="1:13">
+    <row r="283" spans="1:13" hidden="1">
       <c r="A283" s="2">
         <v>281</v>
       </c>
@@ -14600,7 +14598,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="284" spans="1:13">
+    <row r="284" spans="1:13" hidden="1">
       <c r="A284" s="2">
         <v>282</v>
       </c>
@@ -14642,7 +14640,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="285" spans="1:13">
+    <row r="285" spans="1:13" hidden="1">
       <c r="A285" s="2">
         <v>283</v>
       </c>
@@ -14681,7 +14679,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="286" spans="1:13">
+    <row r="286" spans="1:13" hidden="1">
       <c r="A286" s="2">
         <v>284</v>
       </c>
@@ -14720,7 +14718,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="287" spans="1:13">
+    <row r="287" spans="1:13" hidden="1">
       <c r="A287" s="2">
         <v>285</v>
       </c>
@@ -14762,7 +14760,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="288" spans="1:13">
+    <row r="288" spans="1:13" hidden="1">
       <c r="A288" s="2">
         <v>286</v>
       </c>
@@ -14801,7 +14799,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="289" spans="1:13">
+    <row r="289" spans="1:13" hidden="1">
       <c r="A289" s="2">
         <v>287</v>
       </c>
@@ -14843,7 +14841,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="290" spans="1:13">
+    <row r="290" spans="1:13" hidden="1">
       <c r="A290" s="2">
         <v>288</v>
       </c>
@@ -14885,7 +14883,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="291" spans="1:13">
+    <row r="291" spans="1:13" hidden="1">
       <c r="A291" s="2">
         <v>289</v>
       </c>
@@ -14924,7 +14922,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="292" spans="1:13">
+    <row r="292" spans="1:13" hidden="1">
       <c r="A292" s="2">
         <v>290</v>
       </c>
@@ -14966,7 +14964,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="293" spans="1:13">
+    <row r="293" spans="1:13" hidden="1">
       <c r="A293" s="2">
         <v>291</v>
       </c>
@@ -15008,7 +15006,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="294" spans="1:13">
+    <row r="294" spans="1:13" hidden="1">
       <c r="A294" s="2">
         <v>292</v>
       </c>
@@ -15050,7 +15048,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="295" spans="1:13">
+    <row r="295" spans="1:13" hidden="1">
       <c r="A295" s="2">
         <v>293</v>
       </c>
@@ -15092,7 +15090,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="296" spans="1:13">
+    <row r="296" spans="1:13" hidden="1">
       <c r="A296" s="2">
         <v>294</v>
       </c>
@@ -15131,7 +15129,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="297" spans="1:13">
+    <row r="297" spans="1:13" hidden="1">
       <c r="A297" s="2">
         <v>295</v>
       </c>
@@ -15170,7 +15168,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="298" spans="1:13">
+    <row r="298" spans="1:13" hidden="1">
       <c r="A298" s="2">
         <v>296</v>
       </c>
@@ -15209,7 +15207,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="299" spans="1:13">
+    <row r="299" spans="1:13" hidden="1">
       <c r="A299" s="2">
         <v>297</v>
       </c>
@@ -15251,7 +15249,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="300" spans="1:13">
+    <row r="300" spans="1:13" hidden="1">
       <c r="A300" s="2">
         <v>298</v>
       </c>
@@ -15293,7 +15291,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="301" spans="1:13">
+    <row r="301" spans="1:13" hidden="1">
       <c r="A301" s="2">
         <v>299</v>
       </c>
@@ -15332,7 +15330,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="302" spans="1:13">
+    <row r="302" spans="1:13" hidden="1">
       <c r="A302" s="2">
         <v>300</v>
       </c>
@@ -15374,7 +15372,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="303" spans="1:13">
+    <row r="303" spans="1:13" hidden="1">
       <c r="A303" s="2">
         <v>301</v>
       </c>
@@ -15416,7 +15414,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="304" spans="1:13">
+    <row r="304" spans="1:13" hidden="1">
       <c r="A304" s="2">
         <v>302</v>
       </c>
@@ -15455,7 +15453,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="305" spans="1:13">
+    <row r="305" spans="1:13" hidden="1">
       <c r="A305" s="2">
         <v>303</v>
       </c>
@@ -15497,7 +15495,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="306" spans="1:13">
+    <row r="306" spans="1:13" hidden="1">
       <c r="A306" s="2">
         <v>304</v>
       </c>
@@ -15539,7 +15537,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="307" spans="1:13">
+    <row r="307" spans="1:13" hidden="1">
       <c r="A307" s="2">
         <v>305</v>
       </c>
@@ -15578,7 +15576,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="308" spans="1:13">
+    <row r="308" spans="1:13" hidden="1">
       <c r="A308" s="2">
         <v>306</v>
       </c>
@@ -15620,7 +15618,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="309" spans="1:13">
+    <row r="309" spans="1:13" hidden="1">
       <c r="A309" s="2">
         <v>307</v>
       </c>
@@ -15662,7 +15660,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="310" spans="1:13">
+    <row r="310" spans="1:13" hidden="1">
       <c r="A310" s="2">
         <v>308</v>
       </c>
@@ -15701,7 +15699,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="311" spans="1:13">
+    <row r="311" spans="1:13" hidden="1">
       <c r="A311" s="2">
         <v>309</v>
       </c>
@@ -15743,7 +15741,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="312" spans="1:13">
+    <row r="312" spans="1:13" hidden="1">
       <c r="A312" s="2">
         <v>310</v>
       </c>
@@ -15785,7 +15783,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="313" spans="1:13">
+    <row r="313" spans="1:13" hidden="1">
       <c r="A313" s="2">
         <v>311</v>
       </c>
@@ -15824,7 +15822,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="314" spans="1:13">
+    <row r="314" spans="1:13" hidden="1">
       <c r="A314" s="2">
         <v>312</v>
       </c>
@@ -15866,7 +15864,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="315" spans="1:13">
+    <row r="315" spans="1:13" hidden="1">
       <c r="A315" s="2">
         <v>313</v>
       </c>
@@ -15908,7 +15906,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="316" spans="1:13">
+    <row r="316" spans="1:13" hidden="1">
       <c r="A316" s="2">
         <v>314</v>
       </c>
@@ -15947,7 +15945,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="317" spans="1:13">
+    <row r="317" spans="1:13" hidden="1">
       <c r="A317" s="2">
         <v>315</v>
       </c>
@@ -15986,7 +15984,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="318" spans="1:13">
+    <row r="318" spans="1:13" hidden="1">
       <c r="A318" s="2">
         <v>316</v>
       </c>
@@ -16025,7 +16023,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="319" spans="1:13">
+    <row r="319" spans="1:13" hidden="1">
       <c r="A319" s="2">
         <v>317</v>
       </c>
@@ -16067,7 +16065,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="320" spans="1:13">
+    <row r="320" spans="1:13" hidden="1">
       <c r="A320" s="2">
         <v>318</v>
       </c>
@@ -16106,7 +16104,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="321" spans="1:13">
+    <row r="321" spans="1:13" hidden="1">
       <c r="A321" s="2">
         <v>319</v>
       </c>
@@ -16145,7 +16143,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="322" spans="1:13">
+    <row r="322" spans="1:13" hidden="1">
       <c r="A322" s="2">
         <v>320</v>
       </c>
@@ -16184,7 +16182,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="323" spans="1:13">
+    <row r="323" spans="1:13" hidden="1">
       <c r="A323" s="2">
         <v>321</v>
       </c>
@@ -16223,7 +16221,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="324" spans="1:13">
+    <row r="324" spans="1:13" hidden="1">
       <c r="A324" s="2">
         <v>322</v>
       </c>
@@ -16265,7 +16263,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="325" spans="1:13">
+    <row r="325" spans="1:13" hidden="1">
       <c r="A325" s="2">
         <v>323</v>
       </c>
@@ -16307,7 +16305,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="326" spans="1:13">
+    <row r="326" spans="1:13" hidden="1">
       <c r="A326" s="2">
         <v>324</v>
       </c>
@@ -16346,7 +16344,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="327" spans="1:13">
+    <row r="327" spans="1:13" hidden="1">
       <c r="A327" s="2">
         <v>325</v>
       </c>
@@ -16388,7 +16386,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="328" spans="1:13">
+    <row r="328" spans="1:13" hidden="1">
       <c r="A328" s="2">
         <v>326</v>
       </c>
@@ -16430,7 +16428,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="329" spans="1:13">
+    <row r="329" spans="1:13" hidden="1">
       <c r="A329" s="2">
         <v>327</v>
       </c>
@@ -16469,7 +16467,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="330" spans="1:13">
+    <row r="330" spans="1:13" hidden="1">
       <c r="A330" s="2">
         <v>328</v>
       </c>
@@ -16511,7 +16509,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="331" spans="1:13">
+    <row r="331" spans="1:13" hidden="1">
       <c r="A331" s="2">
         <v>329</v>
       </c>
@@ -16553,7 +16551,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="332" spans="1:13">
+    <row r="332" spans="1:13" hidden="1">
       <c r="A332" s="2">
         <v>330</v>
       </c>
@@ -16592,7 +16590,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="333" spans="1:13">
+    <row r="333" spans="1:13" hidden="1">
       <c r="A333" s="2">
         <v>331</v>
       </c>
@@ -16634,7 +16632,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="334" spans="1:13">
+    <row r="334" spans="1:13" hidden="1">
       <c r="A334" s="2">
         <v>332</v>
       </c>
@@ -16676,7 +16674,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="335" spans="1:13">
+    <row r="335" spans="1:13" hidden="1">
       <c r="A335" s="2">
         <v>333</v>
       </c>
@@ -16715,7 +16713,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="336" spans="1:13">
+    <row r="336" spans="1:13" hidden="1">
       <c r="A336" s="2">
         <v>334</v>
       </c>
@@ -16754,7 +16752,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="337" spans="1:13">
+    <row r="337" spans="1:13" hidden="1">
       <c r="A337" s="2">
         <v>335</v>
       </c>
@@ -16797,7 +16795,23 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M337" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <autoFilter ref="A1:M337" xr:uid="{00000000-0009-0000-0000-000002000000}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Early Engagement"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="6">
+      <filters>
+        <filter val="Decision"/>
+        <filter val="Extension"/>
+        <filter val="Finance"/>
+        <filter val="Milestone"/>
+        <filter val="PCP"/>
+        <filter val="Suspension"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="H1:H16 H18:H337">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="END">
       <formula>NOT(ISERROR(SEARCH("END",H1)))</formula>
@@ -16860,7 +16874,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -16889,7 +16903,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -18092,10 +18106,10 @@
   <dimension ref="A1:G257"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B242" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D250" sqref="D250"/>
+      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -18151,7 +18165,7 @@
         <v>296</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G2" s="2">
         <v>1</v>
@@ -18247,7 +18261,7 @@
         <v>302</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>347</v>
+        <v>380</v>
       </c>
       <c r="G6" s="2">
         <v>5</v>
@@ -18295,7 +18309,7 @@
         <v>317</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G8" s="2">
         <v>7</v>
@@ -18319,7 +18333,7 @@
         <v>304</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G9" s="2">
         <v>8</v>
@@ -18343,7 +18357,7 @@
         <v>305</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G10" s="2">
         <v>9</v>
@@ -18367,7 +18381,7 @@
         <v>306</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G11" s="2">
         <v>10</v>
@@ -18391,7 +18405,7 @@
         <v>307</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="G12" s="2">
         <v>11</v>
@@ -18463,7 +18477,7 @@
         <v>308</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G15" s="2">
         <v>14</v>
@@ -18487,7 +18501,7 @@
         <v>309</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G16" s="2">
         <v>15</v>
@@ -18559,7 +18573,7 @@
         <v>310</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G19" s="2">
         <v>18</v>
@@ -18583,7 +18597,7 @@
         <v>311</v>
       </c>
       <c r="F20" s="66" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G20" s="2">
         <v>19</v>
@@ -18607,7 +18621,7 @@
         <v>296</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G21" s="2">
         <v>20</v>
@@ -18631,7 +18645,7 @@
         <v>296</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G22" s="2">
         <v>21</v>
@@ -18679,7 +18693,7 @@
         <v>89</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G24" s="2">
         <v>23</v>
@@ -18703,7 +18717,7 @@
         <v>92</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G25" s="2">
         <v>24</v>
@@ -18727,7 +18741,7 @@
         <v>312</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G26" s="2">
         <v>25</v>
@@ -18751,7 +18765,7 @@
         <v>313</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G27" s="2">
         <v>26</v>
@@ -18775,7 +18789,7 @@
         <v>314</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G28" s="2">
         <v>27</v>
@@ -18796,10 +18810,10 @@
         <v>85</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G29" s="2">
         <v>28</v>
@@ -18820,10 +18834,10 @@
         <v>88</v>
       </c>
       <c r="E30" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>382</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>383</v>
       </c>
       <c r="G30" s="2">
         <v>29</v>
@@ -18847,7 +18861,7 @@
         <v>315</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G31" s="2">
         <v>30</v>
@@ -18895,7 +18909,7 @@
         <v>89</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G33" s="2">
         <v>32</v>
@@ -18919,7 +18933,7 @@
         <v>96</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G34" s="2">
         <v>33</v>
@@ -18943,7 +18957,7 @@
         <v>312</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G35" s="2">
         <v>34</v>
@@ -18991,7 +19005,7 @@
         <v>89</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G37" s="2">
         <v>36</v>
@@ -19015,7 +19029,7 @@
         <v>92</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G38" s="2">
         <v>37</v>
@@ -19039,7 +19053,7 @@
         <v>312</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G39" s="2">
         <v>38</v>
@@ -19063,7 +19077,7 @@
         <v>316</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G40" s="2">
         <v>39</v>
@@ -19087,7 +19101,7 @@
         <v>296</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G41" s="2">
         <v>40</v>
@@ -19111,7 +19125,7 @@
         <v>296</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G42" s="2">
         <v>41</v>
@@ -19135,7 +19149,7 @@
         <v>315</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G43" s="2">
         <v>42</v>
@@ -19183,7 +19197,7 @@
         <v>89</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G45" s="2">
         <v>44</v>
@@ -19207,7 +19221,7 @@
         <v>96</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G46" s="2">
         <v>45</v>
@@ -19231,7 +19245,7 @@
         <v>312</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G47" s="2">
         <v>46</v>
@@ -19279,7 +19293,7 @@
         <v>89</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G49" s="2">
         <v>48</v>
@@ -19303,7 +19317,7 @@
         <v>92</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G50" s="2">
         <v>49</v>
@@ -19327,7 +19341,7 @@
         <v>312</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G51" s="2">
         <v>50</v>
@@ -19351,7 +19365,7 @@
         <v>315</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G52" s="2">
         <v>51</v>
@@ -19399,7 +19413,7 @@
         <v>89</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G54" s="2">
         <v>53</v>
@@ -19423,7 +19437,7 @@
         <v>96</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G55" s="2">
         <v>54</v>
@@ -19447,7 +19461,7 @@
         <v>312</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G56" s="2">
         <v>55</v>
@@ -19495,7 +19509,7 @@
         <v>89</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G58" s="2">
         <v>57</v>
@@ -19519,7 +19533,7 @@
         <v>92</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G59" s="2">
         <v>58</v>
@@ -19543,7 +19557,7 @@
         <v>312</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G60" s="2">
         <v>59</v>
@@ -19564,10 +19578,10 @@
         <v>97</v>
       </c>
       <c r="E61" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="F61" s="70" t="s">
         <v>385</v>
-      </c>
-      <c r="F61" s="70" t="s">
-        <v>386</v>
       </c>
       <c r="G61" s="2">
         <v>60</v>
@@ -19591,7 +19605,7 @@
         <v>318</v>
       </c>
       <c r="F62" s="66" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G62" s="2">
         <v>61</v>
@@ -19615,7 +19629,7 @@
         <v>321</v>
       </c>
       <c r="F63" s="66" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G63" s="2">
         <v>62</v>
@@ -19639,7 +19653,7 @@
         <v>323</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G64" s="2">
         <v>63</v>
@@ -19663,7 +19677,7 @@
         <v>324</v>
       </c>
       <c r="F65" s="66" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G65" s="2">
         <v>64</v>
@@ -19687,7 +19701,7 @@
         <v>325</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G66" s="2">
         <v>65</v>
@@ -19711,7 +19725,7 @@
         <v>326</v>
       </c>
       <c r="F67" s="66" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G67" s="2">
         <v>66</v>
@@ -19735,7 +19749,7 @@
         <v>327</v>
       </c>
       <c r="F68" s="66" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G68" s="2">
         <v>67</v>
@@ -19759,7 +19773,7 @@
         <v>328</v>
       </c>
       <c r="F69" s="66" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G69" s="2">
         <v>68</v>
@@ -19783,7 +19797,7 @@
         <v>333</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G70" s="2">
         <v>69</v>
@@ -19831,7 +19845,7 @@
         <v>89</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G72" s="2">
         <v>71</v>
@@ -19855,7 +19869,7 @@
         <v>96</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G73" s="2">
         <v>72</v>
@@ -19879,7 +19893,7 @@
         <v>312</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G74" s="2">
         <v>73</v>
@@ -19927,7 +19941,7 @@
         <v>89</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G76" s="2">
         <v>75</v>
@@ -19951,7 +19965,7 @@
         <v>92</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G77" s="2">
         <v>76</v>
@@ -19975,7 +19989,7 @@
         <v>312</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G78" s="2">
         <v>77</v>
@@ -19999,7 +20013,7 @@
         <v>89</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G79" s="2">
         <v>78</v>
@@ -20023,7 +20037,7 @@
         <v>96</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G80" s="2">
         <v>79</v>
@@ -20047,7 +20061,7 @@
         <v>312</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G81" s="2">
         <v>80</v>
@@ -20071,7 +20085,7 @@
         <v>329</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G82" s="2">
         <v>81</v>
@@ -20095,7 +20109,7 @@
         <v>330</v>
       </c>
       <c r="F83" s="66" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G83" s="2">
         <v>82</v>
@@ -20143,7 +20157,7 @@
         <v>89</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G85" s="2">
         <v>84</v>
@@ -20167,7 +20181,7 @@
         <v>96</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G86" s="2">
         <v>85</v>
@@ -20191,7 +20205,7 @@
         <v>312</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G87" s="2">
         <v>86</v>
@@ -20239,7 +20253,7 @@
         <v>89</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G89" s="2">
         <v>88</v>
@@ -20263,7 +20277,7 @@
         <v>92</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G90" s="2">
         <v>89</v>
@@ -20287,7 +20301,7 @@
         <v>312</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G91" s="2">
         <v>90</v>
@@ -20308,10 +20322,10 @@
         <v>97</v>
       </c>
       <c r="E92" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="F92" s="1" t="s">
         <v>385</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>386</v>
       </c>
       <c r="G92" s="2">
         <v>91</v>
@@ -20335,7 +20349,7 @@
         <v>318</v>
       </c>
       <c r="F93" s="66" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G93" s="2">
         <v>92</v>
@@ -20359,7 +20373,7 @@
         <v>321</v>
       </c>
       <c r="F94" s="66" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G94" s="2">
         <v>93</v>
@@ -20383,7 +20397,7 @@
         <v>328</v>
       </c>
       <c r="F95" s="66" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G95" s="2">
         <v>94</v>
@@ -20407,7 +20421,7 @@
         <v>333</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G96" s="2">
         <v>95</v>
@@ -20431,7 +20445,7 @@
         <v>331</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G97" s="2">
         <v>96</v>
@@ -20455,7 +20469,7 @@
         <v>332</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G98" s="2">
         <v>97</v>
@@ -20479,7 +20493,7 @@
         <v>333</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G99" s="2">
         <v>98</v>
@@ -20503,7 +20517,7 @@
         <v>315</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G100" s="2">
         <v>99</v>
@@ -20551,7 +20565,7 @@
         <v>89</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G102" s="2">
         <v>101</v>
@@ -20575,7 +20589,7 @@
         <v>96</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G103" s="2">
         <v>102</v>
@@ -20599,7 +20613,7 @@
         <v>312</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G104" s="2">
         <v>103</v>
@@ -20647,7 +20661,7 @@
         <v>89</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G106" s="2">
         <v>105</v>
@@ -20671,7 +20685,7 @@
         <v>92</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G107" s="2">
         <v>106</v>
@@ -20695,7 +20709,7 @@
         <v>312</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G108" s="2">
         <v>107</v>
@@ -20719,7 +20733,7 @@
         <v>334</v>
       </c>
       <c r="F109" s="66" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G109" s="2">
         <v>108</v>
@@ -20743,7 +20757,7 @@
         <v>296</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G110" s="2">
         <v>109</v>
@@ -20767,7 +20781,7 @@
         <v>296</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G111" s="2">
         <v>110</v>
@@ -20791,7 +20805,7 @@
         <v>315</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G112" s="2">
         <v>111</v>
@@ -20839,7 +20853,7 @@
         <v>89</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G114" s="2">
         <v>113</v>
@@ -20863,7 +20877,7 @@
         <v>96</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G115" s="2">
         <v>114</v>
@@ -20887,7 +20901,7 @@
         <v>312</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G116" s="2">
         <v>115</v>
@@ -20935,7 +20949,7 @@
         <v>89</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G118" s="2">
         <v>117</v>
@@ -20959,7 +20973,7 @@
         <v>92</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G119" s="2">
         <v>118</v>
@@ -20983,7 +20997,7 @@
         <v>312</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G120" s="2">
         <v>119</v>
@@ -21007,7 +21021,7 @@
         <v>315</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G121" s="2">
         <v>120</v>
@@ -21055,7 +21069,7 @@
         <v>89</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G123" s="2">
         <v>122</v>
@@ -21079,7 +21093,7 @@
         <v>96</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G124" s="2">
         <v>123</v>
@@ -21103,7 +21117,7 @@
         <v>312</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G125" s="2">
         <v>124</v>
@@ -21151,7 +21165,7 @@
         <v>89</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G127" s="2">
         <v>126</v>
@@ -21175,7 +21189,7 @@
         <v>92</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G128" s="2">
         <v>127</v>
@@ -21199,7 +21213,7 @@
         <v>312</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G129" s="2">
         <v>128</v>
@@ -21223,7 +21237,7 @@
         <v>311</v>
       </c>
       <c r="F130" s="66" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G130" s="2">
         <v>129</v>
@@ -21247,7 +21261,7 @@
         <v>296</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G131" s="2">
         <v>130</v>
@@ -21271,7 +21285,7 @@
         <v>296</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G132" s="2">
         <v>131</v>
@@ -21295,7 +21309,7 @@
         <v>315</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G133" s="2">
         <v>132</v>
@@ -21343,7 +21357,7 @@
         <v>89</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G135" s="2">
         <v>134</v>
@@ -21367,7 +21381,7 @@
         <v>96</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G136" s="2">
         <v>135</v>
@@ -21391,7 +21405,7 @@
         <v>312</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G137" s="2">
         <v>136</v>
@@ -21439,7 +21453,7 @@
         <v>89</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G139" s="2">
         <v>138</v>
@@ -21463,7 +21477,7 @@
         <v>92</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G140" s="2">
         <v>139</v>
@@ -21487,7 +21501,7 @@
         <v>312</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G141" s="2">
         <v>140</v>
@@ -21511,7 +21525,7 @@
         <v>335</v>
       </c>
       <c r="F142" s="66" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G142" s="2">
         <v>141</v>
@@ -21532,10 +21546,10 @@
         <v>85</v>
       </c>
       <c r="E143" s="68" t="s">
+        <v>386</v>
+      </c>
+      <c r="F143" s="1" t="s">
         <v>387</v>
-      </c>
-      <c r="F143" s="1" t="s">
-        <v>388</v>
       </c>
       <c r="G143" s="2">
         <v>142</v>
@@ -21559,7 +21573,7 @@
         <v>336</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G144" s="2">
         <v>143</v>
@@ -21583,7 +21597,7 @@
         <v>315</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G145" s="2">
         <v>144</v>
@@ -21631,7 +21645,7 @@
         <v>89</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G147" s="2">
         <v>146</v>
@@ -21655,7 +21669,7 @@
         <v>96</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G148" s="2">
         <v>147</v>
@@ -21679,7 +21693,7 @@
         <v>312</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G149" s="2">
         <v>148</v>
@@ -21727,7 +21741,7 @@
         <v>89</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G151" s="2">
         <v>150</v>
@@ -21751,7 +21765,7 @@
         <v>92</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G152" s="2">
         <v>151</v>
@@ -21775,7 +21789,7 @@
         <v>312</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G153" s="2">
         <v>152</v>
@@ -21799,7 +21813,7 @@
         <v>339</v>
       </c>
       <c r="F154" s="66" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G154" s="2">
         <v>153</v>
@@ -21847,7 +21861,7 @@
         <v>89</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G156" s="2">
         <v>155</v>
@@ -21871,7 +21885,7 @@
         <v>92</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G157" s="2">
         <v>156</v>
@@ -21895,7 +21909,7 @@
         <v>312</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G158" s="2">
         <v>157</v>
@@ -21919,7 +21933,7 @@
         <v>340</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G159" s="2">
         <v>158</v>
@@ -21943,7 +21957,7 @@
         <v>341</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G160" s="2">
         <v>159</v>
@@ -21967,7 +21981,7 @@
         <v>340</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G161" s="2">
         <v>160</v>
@@ -21991,7 +22005,7 @@
         <v>312</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G162" s="2">
         <v>161</v>
@@ -23265,7 +23279,7 @@
     </row>
     <row r="6" spans="1:59">
       <c r="B6" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>24</v>
@@ -24715,14 +24729,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -24955,21 +24967,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0BEEB2-93D8-45BE-86D5-11172DAC5CD0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37DBE489-EE2E-427D-B9CD-0FAE2F0995FB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
-    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -24994,9 +25005,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37DBE489-EE2E-427D-B9CD-0FAE2F0995FB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0BEEB2-93D8-45BE-86D5-11172DAC5CD0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
+    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
validatae dates removed for testing
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/assessment/002_EAC_Assessment.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/assessment/002_EAC_Assessment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\epic\track\code\epictrack-api\src\api\templates\event_templates\assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0891B01-B3C5-4230-8118-3AB25E6D708C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E1DCBD-ED3F-457B-BD23-5AD012B2EA5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phases" sheetId="1" r:id="rId1"/>
@@ -3113,7 +3113,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D30" sqref="D30"/>
+      <selection pane="bottomRight" activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -16870,11 +16870,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A11" sqref="A11:XFD11"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -17161,6 +17161,7 @@
       <c r="E15" s="2">
         <v>14</v>
       </c>
+      <c r="F15" s="69"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="2">
@@ -18105,11 +18106,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
+      <selection pane="bottomRight" activeCell="A40" sqref="A40:XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -24729,12 +24730,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -24967,20 +24970,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37DBE489-EE2E-427D-B9CD-0FAE2F0995FB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0BEEB2-93D8-45BE-86D5-11172DAC5CD0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
+    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -25005,12 +25009,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0BEEB2-93D8-45BE-86D5-11172DAC5CD0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37DBE489-EE2E-427D-B9CD-0FAE2F0995FB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
-    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
eac_assessment test status updated
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/assessment/002_EAC_Assessment.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/assessment/002_EAC_Assessment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\epic\track\code\epictrack-api\src\api\templates\event_templates\assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E1DCBD-ED3F-457B-BD23-5AD012B2EA5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F123F9C-CE9F-4B5B-B48F-14EF8FE1ACF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1569,7 +1569,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1773,6 +1773,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2086,7 +2089,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2:C13"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -3110,10 +3113,10 @@
   <dimension ref="A1:M337"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B151" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A69" sqref="A69"/>
+      <selection pane="bottomRight" activeCell="D186" sqref="D186:D204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -3171,7 +3174,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" hidden="1">
+    <row r="2" spans="1:13">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3210,7 +3213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" hidden="1">
+    <row r="3" spans="1:13">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3249,7 +3252,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1">
+    <row r="4" spans="1:13">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3330,7 +3333,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" hidden="1">
+    <row r="6" spans="1:13">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3369,7 +3372,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" hidden="1">
+    <row r="7" spans="1:13">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3450,7 +3453,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:13" hidden="1">
+    <row r="9" spans="1:13">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3489,7 +3492,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" hidden="1">
+    <row r="10" spans="1:13">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -3612,7 +3615,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:13" hidden="1">
+    <row r="13" spans="1:13">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -3651,7 +3654,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:13" hidden="1">
+    <row r="14" spans="1:13">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -3693,7 +3696,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:13" hidden="1">
+    <row r="15" spans="1:13">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -3732,7 +3735,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:13" hidden="1">
+    <row r="16" spans="1:13" ht="15" thickBot="1">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -3771,7 +3774,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15" hidden="1" thickBot="1">
+    <row r="17" spans="1:13" ht="15" thickBot="1">
       <c r="A17" s="2">
         <v>9999</v>
       </c>
@@ -3809,7 +3812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:13" hidden="1">
+    <row r="18" spans="1:13">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -6008,7 +6011,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:13" hidden="1">
+    <row r="72" spans="1:13">
       <c r="A72" s="2">
         <v>70</v>
       </c>
@@ -6047,7 +6050,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:13" hidden="1">
+    <row r="73" spans="1:13">
       <c r="A73" s="2">
         <v>71</v>
       </c>
@@ -6128,7 +6131,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:13" hidden="1">
+    <row r="75" spans="1:13">
       <c r="A75" s="2">
         <v>73</v>
       </c>
@@ -6167,7 +6170,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:13" hidden="1">
+    <row r="76" spans="1:13">
       <c r="A76" s="2">
         <v>74</v>
       </c>
@@ -6206,7 +6209,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:13" hidden="1">
+    <row r="77" spans="1:13">
       <c r="A77" s="2">
         <v>75</v>
       </c>
@@ -6248,7 +6251,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:13" hidden="1">
+    <row r="78" spans="1:13">
       <c r="A78" s="2">
         <v>76</v>
       </c>
@@ -6371,7 +6374,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:13" hidden="1">
+    <row r="81" spans="1:13">
       <c r="A81" s="2">
         <v>79</v>
       </c>
@@ -6494,7 +6497,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:13" hidden="1">
+    <row r="84" spans="1:13">
       <c r="A84" s="2">
         <v>82</v>
       </c>
@@ -6617,7 +6620,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:13" hidden="1">
+    <row r="87" spans="1:13">
       <c r="A87" s="2">
         <v>85</v>
       </c>
@@ -6656,7 +6659,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:13" hidden="1">
+    <row r="88" spans="1:13">
       <c r="A88" s="2">
         <v>86</v>
       </c>
@@ -6695,7 +6698,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:13" hidden="1">
+    <row r="89" spans="1:13">
       <c r="A89" s="2">
         <v>87</v>
       </c>
@@ -6818,7 +6821,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:13" hidden="1">
+    <row r="92" spans="1:13">
       <c r="A92" s="2">
         <v>90</v>
       </c>
@@ -6899,7 +6902,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:13" hidden="1">
+    <row r="94" spans="1:13">
       <c r="A94" s="2">
         <v>92</v>
       </c>
@@ -6938,7 +6941,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:13" hidden="1">
+    <row r="95" spans="1:13">
       <c r="A95" s="2">
         <v>93</v>
       </c>
@@ -7019,7 +7022,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:13" hidden="1">
+    <row r="97" spans="1:13">
       <c r="A97" s="2">
         <v>95</v>
       </c>
@@ -7058,7 +7061,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:13" hidden="1">
+    <row r="98" spans="1:13">
       <c r="A98" s="2">
         <v>96</v>
       </c>
@@ -7181,7 +7184,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:13" hidden="1">
+    <row r="101" spans="1:13">
       <c r="A101" s="2">
         <v>99</v>
       </c>
@@ -7304,7 +7307,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:13" hidden="1">
+    <row r="104" spans="1:13">
       <c r="A104" s="2">
         <v>102</v>
       </c>
@@ -7427,7 +7430,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:13" hidden="1">
+    <row r="107" spans="1:13" ht="15" thickBot="1">
       <c r="A107" s="2">
         <v>105</v>
       </c>
@@ -7466,7 +7469,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:13" hidden="1">
+    <row r="108" spans="1:13">
       <c r="A108" s="41">
         <v>106</v>
       </c>
@@ -7506,7 +7509,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:13" ht="15" hidden="1" thickBot="1">
+    <row r="109" spans="1:13" ht="15" thickBot="1">
       <c r="A109" s="42">
         <v>107</v>
       </c>
@@ -7546,7 +7549,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:13" hidden="1">
+    <row r="110" spans="1:13">
       <c r="A110" s="2">
         <v>108</v>
       </c>
@@ -7669,7 +7672,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="113" spans="1:13" hidden="1">
+    <row r="113" spans="1:13">
       <c r="A113" s="2">
         <v>111</v>
       </c>
@@ -7708,7 +7711,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="114" spans="1:13" hidden="1">
+    <row r="114" spans="1:13">
       <c r="A114" s="2">
         <v>112</v>
       </c>
@@ -7747,7 +7750,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="115" spans="1:13" hidden="1">
+    <row r="115" spans="1:13">
       <c r="A115" s="2">
         <v>113</v>
       </c>
@@ -7870,7 +7873,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="118" spans="1:13" hidden="1">
+    <row r="118" spans="1:13">
       <c r="A118" s="2">
         <v>116</v>
       </c>
@@ -7993,7 +7996,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="121" spans="1:13" hidden="1">
+    <row r="121" spans="1:13">
       <c r="A121" s="2">
         <v>119</v>
       </c>
@@ -8032,7 +8035,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="122" spans="1:13" hidden="1">
+    <row r="122" spans="1:13">
       <c r="A122" s="2">
         <v>120</v>
       </c>
@@ -8113,7 +8116,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="124" spans="1:13" hidden="1">
+    <row r="124" spans="1:13">
       <c r="A124" s="2">
         <v>122</v>
       </c>
@@ -8152,7 +8155,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="125" spans="1:13" hidden="1">
+    <row r="125" spans="1:13">
       <c r="A125" s="2">
         <v>123</v>
       </c>
@@ -8191,7 +8194,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="126" spans="1:13" hidden="1">
+    <row r="126" spans="1:13">
       <c r="A126" s="2">
         <v>124</v>
       </c>
@@ -8308,7 +8311,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="129" spans="1:13" hidden="1">
+    <row r="129" spans="1:13">
       <c r="A129" s="2">
         <v>127</v>
       </c>
@@ -8425,7 +8428,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="132" spans="1:13" hidden="1">
+    <row r="132" spans="1:13" ht="15" thickBot="1">
       <c r="A132" s="2">
         <v>130</v>
       </c>
@@ -8464,7 +8467,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="133" spans="1:13" ht="15" hidden="1" thickBot="1">
+    <row r="133" spans="1:13" ht="15" thickBot="1">
       <c r="A133" s="44">
         <v>131</v>
       </c>
@@ -8502,7 +8505,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="134" spans="1:13" hidden="1">
+    <row r="134" spans="1:13">
       <c r="A134" s="2">
         <v>132</v>
       </c>
@@ -8625,7 +8628,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="137" spans="1:13" hidden="1">
+    <row r="137" spans="1:13">
       <c r="A137" s="2">
         <v>135</v>
       </c>
@@ -8664,7 +8667,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="138" spans="1:13" hidden="1">
+    <row r="138" spans="1:13">
       <c r="A138" s="2">
         <v>136</v>
       </c>
@@ -8787,7 +8790,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="141" spans="1:13" hidden="1">
+    <row r="141" spans="1:13">
       <c r="A141" s="2">
         <v>139</v>
       </c>
@@ -8826,7 +8829,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="142" spans="1:13" hidden="1">
+    <row r="142" spans="1:13">
       <c r="A142" s="2">
         <v>140</v>
       </c>
@@ -9033,7 +9036,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="147" spans="1:13" hidden="1">
+    <row r="147" spans="1:13">
       <c r="A147" s="2">
         <v>145</v>
       </c>
@@ -9072,7 +9075,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="148" spans="1:13" hidden="1">
+    <row r="148" spans="1:13">
       <c r="A148" s="2">
         <v>146</v>
       </c>
@@ -9153,7 +9156,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="150" spans="1:13" hidden="1">
+    <row r="150" spans="1:13">
       <c r="A150" s="2">
         <v>148</v>
       </c>
@@ -9192,7 +9195,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="151" spans="1:13" hidden="1">
+    <row r="151" spans="1:13">
       <c r="A151" s="2">
         <v>149</v>
       </c>
@@ -9231,7 +9234,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="152" spans="1:13" hidden="1">
+    <row r="152" spans="1:13">
       <c r="A152" s="2">
         <v>150</v>
       </c>
@@ -9270,7 +9273,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="153" spans="1:13" hidden="1">
+    <row r="153" spans="1:13">
       <c r="A153" s="2">
         <v>151</v>
       </c>
@@ -9309,7 +9312,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="154" spans="1:13" hidden="1">
+    <row r="154" spans="1:13">
       <c r="A154" s="2">
         <v>152</v>
       </c>
@@ -9432,7 +9435,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="157" spans="1:13" hidden="1">
+    <row r="157" spans="1:13">
       <c r="A157" s="2">
         <v>155</v>
       </c>
@@ -9639,7 +9642,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="162" spans="1:13" hidden="1">
+    <row r="162" spans="1:13">
       <c r="A162" s="2">
         <v>160</v>
       </c>
@@ -9678,7 +9681,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="163" spans="1:13" hidden="1">
+    <row r="163" spans="1:13">
       <c r="A163" s="2">
         <v>161</v>
       </c>
@@ -9717,7 +9720,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="164" spans="1:13" hidden="1">
+    <row r="164" spans="1:13">
       <c r="A164" s="2">
         <v>162</v>
       </c>
@@ -9840,7 +9843,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="167" spans="1:13" hidden="1">
+    <row r="167" spans="1:13">
       <c r="A167" s="2">
         <v>165</v>
       </c>
@@ -9963,7 +9966,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="170" spans="1:13" hidden="1">
+    <row r="170" spans="1:13">
       <c r="A170" s="2">
         <v>168</v>
       </c>
@@ -10086,7 +10089,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="173" spans="1:13" hidden="1">
+    <row r="173" spans="1:13">
       <c r="A173" s="2">
         <v>171</v>
       </c>
@@ -10209,7 +10212,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="176" spans="1:13" hidden="1">
+    <row r="176" spans="1:13">
       <c r="A176" s="2">
         <v>174</v>
       </c>
@@ -10332,7 +10335,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="179" spans="1:13" hidden="1">
+    <row r="179" spans="1:13">
       <c r="A179" s="2">
         <v>177</v>
       </c>
@@ -10455,7 +10458,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="182" spans="1:13" hidden="1">
+    <row r="182" spans="1:13">
       <c r="A182" s="2">
         <v>180</v>
       </c>
@@ -10494,7 +10497,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="183" spans="1:13" hidden="1">
+    <row r="183" spans="1:13">
       <c r="A183" s="2">
         <v>181</v>
       </c>
@@ -10617,7 +10620,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="186" spans="1:13" hidden="1">
+    <row r="186" spans="1:13">
       <c r="A186" s="2">
         <v>184</v>
       </c>
@@ -10656,7 +10659,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="187" spans="1:13" hidden="1">
+    <row r="187" spans="1:13">
       <c r="A187" s="2">
         <v>185</v>
       </c>
@@ -10737,7 +10740,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="189" spans="1:13" hidden="1">
+    <row r="189" spans="1:13">
       <c r="A189" s="2">
         <v>187</v>
       </c>
@@ -10776,7 +10779,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="190" spans="1:13" hidden="1">
+    <row r="190" spans="1:13">
       <c r="A190" s="2">
         <v>188</v>
       </c>
@@ -10857,7 +10860,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="192" spans="1:13" hidden="1">
+    <row r="192" spans="1:13">
       <c r="A192" s="2">
         <v>190</v>
       </c>
@@ -10896,7 +10899,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="193" spans="1:13" hidden="1">
+    <row r="193" spans="1:13">
       <c r="A193" s="2">
         <v>191</v>
       </c>
@@ -10938,7 +10941,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="194" spans="1:13" hidden="1">
+    <row r="194" spans="1:13">
       <c r="A194" s="2">
         <v>192</v>
       </c>
@@ -11061,7 +11064,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="197" spans="1:13" hidden="1">
+    <row r="197" spans="1:13">
       <c r="A197" s="2">
         <v>195</v>
       </c>
@@ -11184,7 +11187,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="200" spans="1:13" hidden="1">
+    <row r="200" spans="1:13">
       <c r="A200" s="2">
         <v>198</v>
       </c>
@@ -11307,7 +11310,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="203" spans="1:13" hidden="1">
+    <row r="203" spans="1:13">
       <c r="A203" s="2">
         <v>201</v>
       </c>
@@ -11346,7 +11349,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="204" spans="1:13" hidden="1">
+    <row r="204" spans="1:13">
       <c r="A204" s="2">
         <v>202</v>
       </c>
@@ -11385,7 +11388,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="205" spans="1:13" hidden="1">
+    <row r="205" spans="1:13">
       <c r="A205" s="2">
         <v>203</v>
       </c>
@@ -11508,7 +11511,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="208" spans="1:13" hidden="1">
+    <row r="208" spans="1:13">
       <c r="A208" s="2">
         <v>206</v>
       </c>
@@ -11715,7 +11718,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="213" spans="1:13" hidden="1">
+    <row r="213" spans="1:13">
       <c r="A213" s="2">
         <v>211</v>
       </c>
@@ -11796,7 +11799,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="215" spans="1:13" hidden="1">
+    <row r="215" spans="1:13">
       <c r="A215" s="2">
         <v>213</v>
       </c>
@@ -11877,7 +11880,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="217" spans="1:13" hidden="1">
+    <row r="217" spans="1:13">
       <c r="A217" s="2">
         <v>215</v>
       </c>
@@ -11916,7 +11919,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="218" spans="1:13" hidden="1">
+    <row r="218" spans="1:13">
       <c r="A218" s="2">
         <v>216</v>
       </c>
@@ -11997,7 +12000,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="220" spans="1:13" hidden="1">
+    <row r="220" spans="1:13">
       <c r="A220" s="2">
         <v>218</v>
       </c>
@@ -12120,7 +12123,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="223" spans="1:13" hidden="1">
+    <row r="223" spans="1:13">
       <c r="A223" s="2">
         <v>221</v>
       </c>
@@ -12327,7 +12330,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="228" spans="1:13" hidden="1">
+    <row r="228" spans="1:13">
       <c r="A228" s="2">
         <v>226</v>
       </c>
@@ -12366,7 +12369,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="229" spans="1:13" hidden="1">
+    <row r="229" spans="1:13">
       <c r="A229" s="2">
         <v>227</v>
       </c>
@@ -12405,7 +12408,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="230" spans="1:13" hidden="1">
+    <row r="230" spans="1:13">
       <c r="A230" s="2">
         <v>228</v>
       </c>
@@ -12528,7 +12531,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="233" spans="1:13" hidden="1">
+    <row r="233" spans="1:13">
       <c r="A233" s="2">
         <v>231</v>
       </c>
@@ -12651,7 +12654,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="236" spans="1:13" hidden="1">
+    <row r="236" spans="1:13">
       <c r="A236" s="2">
         <v>234</v>
       </c>
@@ -12774,7 +12777,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="239" spans="1:13" hidden="1">
+    <row r="239" spans="1:13">
       <c r="A239" s="2">
         <v>237</v>
       </c>
@@ -12897,7 +12900,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="242" spans="1:13" hidden="1">
+    <row r="242" spans="1:13">
       <c r="A242" s="2">
         <v>240</v>
       </c>
@@ -13020,7 +13023,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="245" spans="1:13" hidden="1">
+    <row r="245" spans="1:13">
       <c r="A245" s="2">
         <v>243</v>
       </c>
@@ -13143,7 +13146,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="248" spans="1:13" hidden="1">
+    <row r="248" spans="1:13">
       <c r="A248" s="2">
         <v>246</v>
       </c>
@@ -13182,7 +13185,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="249" spans="1:13" hidden="1">
+    <row r="249" spans="1:13">
       <c r="A249" s="2">
         <v>247</v>
       </c>
@@ -13305,7 +13308,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="252" spans="1:13" hidden="1">
+    <row r="252" spans="1:13">
       <c r="A252" s="2">
         <v>250</v>
       </c>
@@ -13344,7 +13347,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="253" spans="1:13" hidden="1">
+    <row r="253" spans="1:13">
       <c r="A253" s="2">
         <v>251</v>
       </c>
@@ -13383,7 +13386,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="254" spans="1:13" hidden="1">
+    <row r="254" spans="1:13">
       <c r="A254" s="2">
         <v>252</v>
       </c>
@@ -13464,7 +13467,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="256" spans="1:13" hidden="1">
+    <row r="256" spans="1:13">
       <c r="A256" s="2">
         <v>254</v>
       </c>
@@ -13503,7 +13506,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="257" spans="1:13" hidden="1">
+    <row r="257" spans="1:13">
       <c r="A257" s="2">
         <v>255</v>
       </c>
@@ -13584,7 +13587,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="259" spans="1:13" hidden="1">
+    <row r="259" spans="1:13">
       <c r="A259" s="2">
         <v>257</v>
       </c>
@@ -13623,7 +13626,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="260" spans="1:13" hidden="1">
+    <row r="260" spans="1:13">
       <c r="A260" s="2">
         <v>258</v>
       </c>
@@ -13665,7 +13668,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="261" spans="1:13" hidden="1">
+    <row r="261" spans="1:13">
       <c r="A261" s="2">
         <v>259</v>
       </c>
@@ -13788,7 +13791,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="264" spans="1:13" hidden="1">
+    <row r="264" spans="1:13">
       <c r="A264" s="2">
         <v>262</v>
       </c>
@@ -13911,7 +13914,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="267" spans="1:13" hidden="1">
+    <row r="267" spans="1:13">
       <c r="A267" s="2">
         <v>265</v>
       </c>
@@ -14034,7 +14037,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="270" spans="1:13" hidden="1">
+    <row r="270" spans="1:13">
       <c r="A270" s="2">
         <v>268</v>
       </c>
@@ -14073,7 +14076,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="271" spans="1:13" hidden="1">
+    <row r="271" spans="1:13">
       <c r="A271" s="2">
         <v>269</v>
       </c>
@@ -14190,7 +14193,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="274" spans="1:13" hidden="1">
+    <row r="274" spans="1:13">
       <c r="A274" s="2">
         <v>272</v>
       </c>
@@ -14313,7 +14316,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="277" spans="1:13" hidden="1">
+    <row r="277" spans="1:13">
       <c r="A277" s="2">
         <v>275</v>
       </c>
@@ -14352,7 +14355,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="278" spans="1:13" hidden="1">
+    <row r="278" spans="1:13">
       <c r="A278" s="2">
         <v>276</v>
       </c>
@@ -14559,7 +14562,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="283" spans="1:13" hidden="1">
+    <row r="283" spans="1:13">
       <c r="A283" s="2">
         <v>281</v>
       </c>
@@ -14640,7 +14643,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="285" spans="1:13" hidden="1">
+    <row r="285" spans="1:13">
       <c r="A285" s="2">
         <v>283</v>
       </c>
@@ -14679,7 +14682,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="286" spans="1:13" hidden="1">
+    <row r="286" spans="1:13">
       <c r="A286" s="2">
         <v>284</v>
       </c>
@@ -14760,7 +14763,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="288" spans="1:13" hidden="1">
+    <row r="288" spans="1:13">
       <c r="A288" s="2">
         <v>286</v>
       </c>
@@ -14883,7 +14886,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="291" spans="1:13" hidden="1">
+    <row r="291" spans="1:13">
       <c r="A291" s="2">
         <v>289</v>
       </c>
@@ -15090,7 +15093,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="296" spans="1:13" hidden="1">
+    <row r="296" spans="1:13">
       <c r="A296" s="2">
         <v>294</v>
       </c>
@@ -15129,7 +15132,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="297" spans="1:13" hidden="1">
+    <row r="297" spans="1:13">
       <c r="A297" s="2">
         <v>295</v>
       </c>
@@ -15168,7 +15171,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="298" spans="1:13" hidden="1">
+    <row r="298" spans="1:13">
       <c r="A298" s="2">
         <v>296</v>
       </c>
@@ -15291,7 +15294,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="301" spans="1:13" hidden="1">
+    <row r="301" spans="1:13">
       <c r="A301" s="2">
         <v>299</v>
       </c>
@@ -15414,7 +15417,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="304" spans="1:13" hidden="1">
+    <row r="304" spans="1:13">
       <c r="A304" s="2">
         <v>302</v>
       </c>
@@ -15537,7 +15540,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="307" spans="1:13" hidden="1">
+    <row r="307" spans="1:13">
       <c r="A307" s="2">
         <v>305</v>
       </c>
@@ -15660,7 +15663,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="310" spans="1:13" hidden="1">
+    <row r="310" spans="1:13">
       <c r="A310" s="2">
         <v>308</v>
       </c>
@@ -15783,7 +15786,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="313" spans="1:13" hidden="1">
+    <row r="313" spans="1:13">
       <c r="A313" s="2">
         <v>311</v>
       </c>
@@ -15906,7 +15909,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="316" spans="1:13" hidden="1">
+    <row r="316" spans="1:13">
       <c r="A316" s="2">
         <v>314</v>
       </c>
@@ -15945,7 +15948,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="317" spans="1:13" hidden="1">
+    <row r="317" spans="1:13">
       <c r="A317" s="2">
         <v>315</v>
       </c>
@@ -15984,7 +15987,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="318" spans="1:13" hidden="1">
+    <row r="318" spans="1:13">
       <c r="A318" s="2">
         <v>316</v>
       </c>
@@ -16065,7 +16068,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="320" spans="1:13" hidden="1">
+    <row r="320" spans="1:13">
       <c r="A320" s="2">
         <v>318</v>
       </c>
@@ -16104,7 +16107,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="321" spans="1:13" hidden="1">
+    <row r="321" spans="1:13">
       <c r="A321" s="2">
         <v>319</v>
       </c>
@@ -16143,7 +16146,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="322" spans="1:13" hidden="1">
+    <row r="322" spans="1:13">
       <c r="A322" s="2">
         <v>320</v>
       </c>
@@ -16182,7 +16185,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="323" spans="1:13" hidden="1">
+    <row r="323" spans="1:13">
       <c r="A323" s="2">
         <v>321</v>
       </c>
@@ -16305,7 +16308,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="326" spans="1:13" hidden="1">
+    <row r="326" spans="1:13">
       <c r="A326" s="2">
         <v>324</v>
       </c>
@@ -16428,7 +16431,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="329" spans="1:13" hidden="1">
+    <row r="329" spans="1:13">
       <c r="A329" s="2">
         <v>327</v>
       </c>
@@ -16551,7 +16554,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="332" spans="1:13" hidden="1">
+    <row r="332" spans="1:13">
       <c r="A332" s="2">
         <v>330</v>
       </c>
@@ -16674,7 +16677,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="335" spans="1:13" hidden="1">
+    <row r="335" spans="1:13">
       <c r="A335" s="2">
         <v>333</v>
       </c>
@@ -16713,7 +16716,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="336" spans="1:13" hidden="1">
+    <row r="336" spans="1:13">
       <c r="A336" s="2">
         <v>334</v>
       </c>
@@ -16796,11 +16799,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:M337" xr:uid="{00000000-0009-0000-0000-000002000000}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Early Engagement"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="6">
       <filters>
         <filter val="Decision"/>
@@ -16871,10 +16869,10 @@
   <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomRight" activeCell="F37" sqref="D37:F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -16923,6 +16921,7 @@
       <c r="E2" s="2">
         <v>1</v>
       </c>
+      <c r="F2" s="69"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
@@ -16941,6 +16940,7 @@
       <c r="E3" s="2">
         <v>2</v>
       </c>
+      <c r="F3" s="69"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2">
@@ -16959,6 +16959,7 @@
       <c r="E4" s="2">
         <v>3</v>
       </c>
+      <c r="F4" s="69"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2">
@@ -16977,6 +16978,7 @@
       <c r="E5" s="2">
         <v>4</v>
       </c>
+      <c r="F5" s="69"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2">
@@ -17014,6 +17016,7 @@
       <c r="E7" s="2">
         <v>6</v>
       </c>
+      <c r="F7" s="69"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2">
@@ -17032,6 +17035,7 @@
       <c r="E8" s="2">
         <v>7</v>
       </c>
+      <c r="F8" s="69"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2">
@@ -17107,6 +17111,7 @@
       <c r="E12" s="2">
         <v>11</v>
       </c>
+      <c r="F12" s="71"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="2">
@@ -17125,6 +17130,7 @@
       <c r="E13" s="2">
         <v>12</v>
       </c>
+      <c r="F13" s="69"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="2">
@@ -17143,6 +17149,7 @@
       <c r="E14" s="2">
         <v>13</v>
       </c>
+      <c r="F14" s="69"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="2">
@@ -17180,6 +17187,7 @@
       <c r="E16" s="2">
         <v>15</v>
       </c>
+      <c r="F16" s="69"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2">
@@ -17198,6 +17206,7 @@
       <c r="E17" s="2">
         <v>16</v>
       </c>
+      <c r="F17" s="69"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2">
@@ -17216,6 +17225,7 @@
       <c r="E18" s="2">
         <v>17</v>
       </c>
+      <c r="F18" s="71"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2">
@@ -17234,6 +17244,7 @@
       <c r="E19" s="2">
         <v>18</v>
       </c>
+      <c r="F19" s="69"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2">
@@ -17252,6 +17263,7 @@
       <c r="E20" s="2">
         <v>19</v>
       </c>
+      <c r="F20" s="69"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2">
@@ -17270,6 +17282,7 @@
       <c r="E21" s="2">
         <v>20</v>
       </c>
+      <c r="F21" s="71"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="2">
@@ -17307,6 +17320,7 @@
       <c r="E23" s="2">
         <v>22</v>
       </c>
+      <c r="F23" s="69"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="2">
@@ -17363,6 +17377,7 @@
       <c r="E26" s="2">
         <v>25</v>
       </c>
+      <c r="F26" s="69"/>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="2">
@@ -17381,6 +17396,7 @@
       <c r="E27" s="2">
         <v>26</v>
       </c>
+      <c r="F27" s="69"/>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="2">
@@ -17399,6 +17415,7 @@
       <c r="E28" s="2">
         <v>27</v>
       </c>
+      <c r="F28" s="69"/>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="2">
@@ -17417,6 +17434,7 @@
       <c r="E29" s="2">
         <v>28</v>
       </c>
+      <c r="F29" s="69"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="2">
@@ -17435,6 +17453,7 @@
       <c r="E30" s="2">
         <v>29</v>
       </c>
+      <c r="F30" s="69"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="2">
@@ -17453,6 +17472,7 @@
       <c r="E31" s="2">
         <v>30</v>
       </c>
+      <c r="F31" s="69"/>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="2">
@@ -17471,8 +17491,9 @@
       <c r="E32" s="2">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32" s="69"/>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -17489,8 +17510,9 @@
       <c r="E33" s="2">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33" s="69"/>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -17507,8 +17529,9 @@
       <c r="E34" s="2">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34" s="69"/>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -17525,8 +17548,9 @@
       <c r="E35" s="2">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35" s="69"/>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -17543,8 +17567,9 @@
       <c r="E36" s="2">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36" s="69"/>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -17562,7 +17587,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:6">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -17580,7 +17605,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:6">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -17597,8 +17622,9 @@
       <c r="E39" s="2">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39" s="69"/>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -17615,8 +17641,9 @@
       <c r="E40" s="2">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="F40" s="71"/>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -17633,8 +17660,9 @@
       <c r="E41" s="2">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="F41" s="69"/>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -17651,8 +17679,9 @@
       <c r="E42" s="2">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="F42" s="69"/>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -17669,8 +17698,9 @@
       <c r="E43" s="2">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="F43" s="69"/>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -17687,8 +17717,9 @@
       <c r="E44" s="2">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="F44" s="69"/>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -17705,8 +17736,9 @@
       <c r="E45" s="2">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="F45" s="69"/>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -17723,8 +17755,9 @@
       <c r="E46" s="2">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="F46" s="71"/>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -17741,8 +17774,9 @@
       <c r="E47" s="2">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="F47" s="69"/>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -17759,8 +17793,9 @@
       <c r="E48" s="2">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="F48" s="69"/>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -17777,8 +17812,9 @@
       <c r="E49" s="2">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="F49" s="71"/>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -17795,8 +17831,9 @@
       <c r="E50" s="2">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="F50" s="69"/>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -17813,8 +17850,9 @@
       <c r="E51" s="2">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="F51" s="69"/>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -17831,8 +17869,9 @@
       <c r="E52" s="2">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="F52" s="69"/>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -17849,8 +17888,9 @@
       <c r="E53" s="2">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="F53" s="69"/>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -17867,8 +17907,9 @@
       <c r="E54" s="2">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="F54" s="69"/>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -17885,8 +17926,9 @@
       <c r="E55" s="2">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="F55" s="71"/>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -17903,8 +17945,9 @@
       <c r="E56" s="2">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="F56" s="69"/>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -17921,8 +17964,9 @@
       <c r="E57" s="2">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="F57" s="69"/>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -17939,8 +17983,9 @@
       <c r="E58" s="2">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="F58" s="69"/>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -17957,8 +18002,9 @@
       <c r="E59" s="2">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="F59" s="69"/>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -17975,8 +18021,9 @@
       <c r="E60" s="2">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="F60" s="71"/>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -17993,8 +18040,9 @@
       <c r="E61" s="2">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:5">
+      <c r="F61" s="69"/>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -18011,8 +18059,9 @@
       <c r="E62" s="2">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:5">
+      <c r="F62" s="69"/>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -18029,8 +18078,9 @@
       <c r="E63" s="2">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:5">
+      <c r="F63" s="69"/>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -18047,8 +18097,9 @@
       <c r="E64" s="2">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:5">
+      <c r="F64" s="69"/>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -18065,8 +18116,9 @@
       <c r="E65" s="2">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:5">
+      <c r="F65" s="69"/>
+    </row>
+    <row r="66" spans="1:6">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -18083,6 +18135,7 @@
       <c r="E66" s="2">
         <v>65</v>
       </c>
+      <c r="F66" s="69"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E15" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
@@ -18107,10 +18160,10 @@
   <dimension ref="A1:G257"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B86" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A40" sqref="A40:XFD40"/>
+      <selection pane="bottomRight" activeCell="A99" sqref="A99:XFD99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -24730,14 +24783,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -24970,21 +25021,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0BEEB2-93D8-45BE-86D5-11172DAC5CD0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37DBE489-EE2E-427D-B9CD-0FAE2F0995FB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
-    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -25009,9 +25059,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37DBE489-EE2E-427D-B9CD-0FAE2F0995FB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0BEEB2-93D8-45BE-86D5-11172DAC5CD0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
+    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
should be able to filter work as active/inactive/all
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/assessment/002_EAC_Assessment.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/assessment/002_EAC_Assessment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\epic\track\code\epictrack-api\src\api\templates\event_templates\assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB68491-F4FF-47AD-9CB0-23697C731E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896C0D24-AFBE-498A-A83E-F2AA80F017AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29940" yWindow="1140" windowWidth="21600" windowHeight="11175" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phases" sheetId="1" r:id="rId1"/>
@@ -3112,11 +3112,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:M337"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B151" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D186" sqref="D186:D204"/>
+      <selection pane="bottomRight" activeCell="K97" sqref="K97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -7055,7 +7055,7 @@
         <v>0</v>
       </c>
       <c r="L97" s="2" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="M97" s="2">
         <v>95</v>
@@ -16868,8 +16868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="G43" sqref="G43"/>
@@ -24783,14 +24783,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -25023,21 +25021,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0BEEB2-93D8-45BE-86D5-11172DAC5CD0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37DBE489-EE2E-427D-B9CD-0FAE2F0995FB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
-    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -25062,9 +25059,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37DBE489-EE2E-427D-B9CD-0FAE2F0995FB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0BEEB2-93D8-45BE-86D5-11172DAC5CD0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
+    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
should be able to filter work as active/inactive/all (#2130)
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/assessment/002_EAC_Assessment.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/assessment/002_EAC_Assessment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\epic\track\code\epictrack-api\src\api\templates\event_templates\assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB68491-F4FF-47AD-9CB0-23697C731E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896C0D24-AFBE-498A-A83E-F2AA80F017AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29940" yWindow="1140" windowWidth="21600" windowHeight="11175" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phases" sheetId="1" r:id="rId1"/>
@@ -3112,11 +3112,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:M337"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B151" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D186" sqref="D186:D204"/>
+      <selection pane="bottomRight" activeCell="K97" sqref="K97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -7055,7 +7055,7 @@
         <v>0</v>
       </c>
       <c r="L97" s="2" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="M97" s="2">
         <v>95</v>
@@ -16868,8 +16868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="G43" sqref="G43"/>
@@ -24783,14 +24783,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -25023,21 +25021,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0BEEB2-93D8-45BE-86D5-11172DAC5CD0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37DBE489-EE2E-427D-B9CD-0FAE2F0995FB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
-    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -25062,9 +25059,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37DBE489-EE2E-427D-B9CD-0FAE2F0995FB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0BEEB2-93D8-45BE-86D5-11172DAC5CD0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
+    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Dispute Resolution - NONE
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/assessment/002_EAC_Assessment.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/assessment/002_EAC_Assessment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\epic\track\code\epictrack-api\src\api\templates\event_templates\assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896C0D24-AFBE-498A-A83E-F2AA80F017AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9AD25D-A25D-4207-95F2-85F617FB95E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29940" yWindow="1140" windowWidth="21600" windowHeight="11175" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phases" sheetId="1" r:id="rId1"/>
@@ -3112,7 +3112,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:M337"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="E81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -18159,11 +18159,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G257"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B86" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A99" sqref="A99:XFD99"/>
+      <selection pane="bottomRight" activeCell="D31" sqref="D31:D145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -18909,7 +18909,7 @@
         <v>A Matter has been Referred for Dispute Resolution</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>95</v>
+        <v>295</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>315</v>
@@ -19197,7 +19197,7 @@
         <v>A Matter has been Referred for Dispute Resolution</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>95</v>
+        <v>295</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>315</v>
@@ -19413,7 +19413,7 @@
         <v>A Matter has been Referred for Dispute Resolution</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>95</v>
+        <v>295</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>315</v>
@@ -20565,7 +20565,7 @@
         <v>A Matter has been Referred for Dispute Resolution</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>95</v>
+        <v>295</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>315</v>
@@ -20853,7 +20853,7 @@
         <v>A Matter has been Referred for Dispute Resolution</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>95</v>
+        <v>295</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>315</v>
@@ -21069,7 +21069,7 @@
         <v>A Matter has been Referred for Dispute Resolution</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>95</v>
+        <v>295</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>315</v>
@@ -21357,7 +21357,7 @@
         <v>A Matter has been Referred for Dispute Resolution</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>95</v>
+        <v>295</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>315</v>
@@ -21645,7 +21645,7 @@
         <v>A Matter has been Referred for Dispute Resolution</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>95</v>
+        <v>295</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>315</v>
@@ -24783,12 +24783,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -25021,20 +25023,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37DBE489-EE2E-427D-B9CD-0FAE2F0995FB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0BEEB2-93D8-45BE-86D5-11172DAC5CD0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
+    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -25059,12 +25062,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0BEEB2-93D8-45BE-86D5-11172DAC5CD0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37DBE489-EE2E-427D-B9CD-0FAE2F0995FB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
-    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Decision maker change (#2169)
* Dispute Resolution - NONE

* decision maker change in event form

* lintfix

* lintfix
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/assessment/002_EAC_Assessment.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/assessment/002_EAC_Assessment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\epic\track\code\epictrack-api\src\api\templates\event_templates\assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896C0D24-AFBE-498A-A83E-F2AA80F017AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9AD25D-A25D-4207-95F2-85F617FB95E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29940" yWindow="1140" windowWidth="21600" windowHeight="11175" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phases" sheetId="1" r:id="rId1"/>
@@ -3112,7 +3112,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:M337"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="E81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -18159,11 +18159,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G257"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B86" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A99" sqref="A99:XFD99"/>
+      <selection pane="bottomRight" activeCell="D31" sqref="D31:D145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -18909,7 +18909,7 @@
         <v>A Matter has been Referred for Dispute Resolution</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>95</v>
+        <v>295</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>315</v>
@@ -19197,7 +19197,7 @@
         <v>A Matter has been Referred for Dispute Resolution</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>95</v>
+        <v>295</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>315</v>
@@ -19413,7 +19413,7 @@
         <v>A Matter has been Referred for Dispute Resolution</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>95</v>
+        <v>295</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>315</v>
@@ -20565,7 +20565,7 @@
         <v>A Matter has been Referred for Dispute Resolution</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>95</v>
+        <v>295</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>315</v>
@@ -20853,7 +20853,7 @@
         <v>A Matter has been Referred for Dispute Resolution</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>95</v>
+        <v>295</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>315</v>
@@ -21069,7 +21069,7 @@
         <v>A Matter has been Referred for Dispute Resolution</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>95</v>
+        <v>295</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>315</v>
@@ -21357,7 +21357,7 @@
         <v>A Matter has been Referred for Dispute Resolution</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>95</v>
+        <v>295</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>315</v>
@@ -21645,7 +21645,7 @@
         <v>A Matter has been Referred for Dispute Resolution</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>95</v>
+        <v>295</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>315</v>
@@ -24783,12 +24783,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -25021,20 +25023,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37DBE489-EE2E-427D-B9CD-0FAE2F0995FB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0BEEB2-93D8-45BE-86D5-11172DAC5CD0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
+    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -25059,12 +25062,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0BEEB2-93D8-45BE-86D5-11172DAC5CD0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37DBE489-EE2E-427D-B9CD-0FAE2F0995FB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
-    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>